<commit_message>
Maj planning contenu et product backlog
</commit_message>
<xml_diff>
--- a/Documents/0_Planning.xlsx
+++ b/Documents/0_Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBC6C0E-CB19-4C74-98E9-B6DF465E462F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D28C6C7-427A-4BEE-86B1-591F50367233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -126,9 +126,6 @@
     <t>Projet "WavContact"</t>
   </si>
   <si>
-    <t>Etude d'opportunité</t>
-  </si>
-  <si>
     <t>Réunion avec le mandant</t>
   </si>
   <si>
@@ -142,12 +139,6 @@
   </si>
   <si>
     <t>PV réunion A0</t>
-  </si>
-  <si>
-    <t>Révision de l'étude d'opportunité</t>
-  </si>
-  <si>
-    <t>Etude des besoins du mandant</t>
   </si>
   <si>
     <t>Réunion A1</t>
@@ -237,12 +228,6 @@
     <t>Reddition à 12h00</t>
   </si>
   <si>
-    <t xml:space="preserve">Mise en place du login </t>
-  </si>
-  <si>
-    <t>Document : Plan d'Assurance Qualité</t>
-  </si>
-  <si>
     <t>PV réunion A2.1</t>
   </si>
   <si>
@@ -258,22 +243,7 @@
     <t>CC, AM</t>
   </si>
   <si>
-    <t>Création et insertion de la base de donnée</t>
-  </si>
-  <si>
-    <t>Réalisation des maquettes V2 sur VisualStudio</t>
-  </si>
-  <si>
     <t>CC, (CH), AM, (AS)</t>
-  </si>
-  <si>
-    <t>Finalisation des maquettes sur VisualStudio</t>
-  </si>
-  <si>
-    <t>Recherche sécurité, loi, etc</t>
-  </si>
-  <si>
-    <t>Création base de données pour le matériel</t>
   </si>
   <si>
     <t>CH, CC, AM</t>
@@ -354,13 +324,7 @@
     <t>Sprint 5 (avec ± 2 semaines de vacances de février)</t>
   </si>
   <si>
-    <t>Création base de données WavMap</t>
-  </si>
-  <si>
     <t>CC</t>
-  </si>
-  <si>
-    <t>Recherche API WavMap</t>
   </si>
   <si>
     <t>AM</t>
@@ -378,25 +342,61 @@
     <t>Continuation code Visual Studio</t>
   </si>
   <si>
-    <t>Documentation manuel utilisation</t>
-  </si>
-  <si>
-    <t>Création des maquettes de WavCom</t>
-  </si>
-  <si>
-    <t>Création de la modélisation de WavCom</t>
-  </si>
-  <si>
-    <t>Finalisation de la modélisation simple de WavCom</t>
-  </si>
-  <si>
-    <t>Finalisation de la maquette simple de WavCom</t>
-  </si>
-  <si>
     <t>Modélisation BDD de WavCom</t>
   </si>
   <si>
     <t>Maquettes sur Visual Studio de WavCom</t>
+  </si>
+  <si>
+    <t>Document étude des besoins du mandant</t>
+  </si>
+  <si>
+    <t>Modélisation de l'application de WavCom</t>
+  </si>
+  <si>
+    <t>Document étude d'opportunité et liste des risques</t>
+  </si>
+  <si>
+    <t>Révision de l'étude d'opportunité et de la liste des risques</t>
+  </si>
+  <si>
+    <t>Maquettes sur papier de WavCom</t>
+  </si>
+  <si>
+    <t>Document Plan d'Assurance Qualité</t>
+  </si>
+  <si>
+    <t>Révision des maquettes sur VisualStudio</t>
+  </si>
+  <si>
+    <t>Recherche sécurité, loi, etc.</t>
+  </si>
+  <si>
+    <t>Base de donnée de WavCom</t>
+  </si>
+  <si>
+    <t>Document de vision</t>
+  </si>
+  <si>
+    <t>Mise en place du login sur WavCom</t>
+  </si>
+  <si>
+    <t>Base de donnée de gestion de matériel pour WavCom</t>
+  </si>
+  <si>
+    <t>Recherche API pour la carte de WavMap</t>
+  </si>
+  <si>
+    <t>Base de données WavMap</t>
+  </si>
+  <si>
+    <t>Documentation manuel utilisateur</t>
+  </si>
+  <si>
+    <t>Finalisation des maquettes sur VisualStudio pour WavCom</t>
+  </si>
+  <si>
+    <t>Documentation des jeux de tests</t>
   </si>
 </sst>
 </file>
@@ -1228,6 +1228,7 @@
     <xf numFmtId="168" fontId="24" fillId="37" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1249,7 +1250,6 @@
     <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20 % - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1307,37 +1307,7 @@
     <cellStyle name="Vérification" xfId="25" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zTexteMasqué" xfId="3" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="60">
     <dxf>
       <fill>
         <patternFill>
@@ -1944,15 +1914,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListeTâches" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="62"/>
-      <tableStyleElement type="headerRow" dxfId="61"/>
-      <tableStyleElement type="totalRow" dxfId="60"/>
-      <tableStyleElement type="firstColumn" dxfId="59"/>
-      <tableStyleElement type="lastColumn" dxfId="58"/>
-      <tableStyleElement type="firstRowStripe" dxfId="57"/>
-      <tableStyleElement type="secondRowStripe" dxfId="56"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="55"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="54"/>
+      <tableStyleElement type="wholeTable" dxfId="59"/>
+      <tableStyleElement type="headerRow" dxfId="58"/>
+      <tableStyleElement type="totalRow" dxfId="57"/>
+      <tableStyleElement type="firstColumn" dxfId="56"/>
+      <tableStyleElement type="lastColumn" dxfId="55"/>
+      <tableStyleElement type="firstRowStripe" dxfId="54"/>
+      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="52"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="51"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2311,11 +2281,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL80"/>
+  <dimension ref="A1:BL82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="7" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2347,8 +2317,8 @@
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="19"/>
-      <c r="B2" s="44" t="s">
-        <v>32</v>
+      <c r="B2" s="45" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -2359,7 +2329,7 @@
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="19"/>
-      <c r="B3" s="44"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="4"/>
@@ -2371,118 +2341,118 @@
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47">
+      <c r="D4" s="47"/>
+      <c r="E4" s="48">
         <v>44459</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="31">
         <v>23</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="42">
         <f>I6</f>
         <v>44613</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="41">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="42">
         <f>P6</f>
         <v>44620</v>
       </c>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="41">
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="42">
         <f>W6</f>
         <v>44627</v>
       </c>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="41">
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="42">
         <f>AD6</f>
         <v>44634</v>
       </c>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="42"/>
-      <c r="AH5" s="42"/>
-      <c r="AI5" s="42"/>
-      <c r="AJ5" s="43"/>
-      <c r="AK5" s="41">
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="43"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="42">
         <f>AK6</f>
         <v>44641</v>
       </c>
-      <c r="AL5" s="42"/>
-      <c r="AM5" s="42"/>
-      <c r="AN5" s="42"/>
-      <c r="AO5" s="42"/>
-      <c r="AP5" s="42"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="41">
+      <c r="AL5" s="43"/>
+      <c r="AM5" s="43"/>
+      <c r="AN5" s="43"/>
+      <c r="AO5" s="43"/>
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="44"/>
+      <c r="AR5" s="42">
         <f>AR6</f>
         <v>44648</v>
       </c>
-      <c r="AS5" s="42"/>
-      <c r="AT5" s="42"/>
-      <c r="AU5" s="42"/>
-      <c r="AV5" s="42"/>
-      <c r="AW5" s="42"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="41">
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="43"/>
+      <c r="AV5" s="43"/>
+      <c r="AW5" s="43"/>
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="42">
         <f>AY6</f>
         <v>44655</v>
       </c>
-      <c r="AZ5" s="42"/>
-      <c r="BA5" s="42"/>
-      <c r="BB5" s="42"/>
-      <c r="BC5" s="42"/>
-      <c r="BD5" s="42"/>
-      <c r="BE5" s="43"/>
-      <c r="BF5" s="41">
+      <c r="AZ5" s="43"/>
+      <c r="BA5" s="43"/>
+      <c r="BB5" s="43"/>
+      <c r="BC5" s="43"/>
+      <c r="BD5" s="43"/>
+      <c r="BE5" s="44"/>
+      <c r="BF5" s="42">
         <f>BF6</f>
         <v>44662</v>
       </c>
-      <c r="BG5" s="42"/>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="42"/>
-      <c r="BJ5" s="42"/>
-      <c r="BK5" s="42"/>
-      <c r="BL5" s="43"/>
+      <c r="BG5" s="43"/>
+      <c r="BH5" s="43"/>
+      <c r="BI5" s="43"/>
+      <c r="BJ5" s="43"/>
+      <c r="BK5" s="43"/>
+      <c r="BL5" s="44"/>
     </row>
     <row r="6" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="I6" s="26">
         <f>Début_Projet-WEEKDAY(Début_Projet,1)+2+7*(Semaine_Affichage-1)</f>
         <v>44613</v>
@@ -2961,7 +2931,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
@@ -2969,7 +2939,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H77" si="4">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
+        <f t="shared" ref="H8:H79" si="4">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
         <v/>
       </c>
       <c r="I8" s="15"/>
@@ -3034,10 +3004,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="35">
         <v>1</v>
@@ -3116,10 +3086,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" s="14">
         <v>1</v>
@@ -3197,10 +3167,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="18"/>
       <c r="B11" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="14">
         <v>1</v>
@@ -3278,10 +3248,10 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19"/>
       <c r="B12" s="24" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="14">
         <v>1</v>
@@ -3359,10 +3329,10 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18"/>
       <c r="B13" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="14">
         <v>1</v>
@@ -3440,10 +3410,10 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="18"/>
       <c r="B14" s="33" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14" s="35">
         <v>1</v>
@@ -3521,10 +3491,10 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="18"/>
       <c r="B15" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="14">
         <v>1</v>
@@ -3602,10 +3572,10 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="18"/>
       <c r="B16" s="24" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
@@ -3685,7 +3655,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="39"/>
@@ -3756,10 +3726,10 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18"/>
       <c r="B18" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="D18" s="14">
         <v>1</v>
@@ -3837,10 +3807,10 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="18"/>
       <c r="B19" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D19" s="14">
         <v>1</v>
@@ -3850,14 +3820,11 @@
         <v>44478</v>
       </c>
       <c r="F19" s="29">
-        <f>E19+7</f>
-        <v>44485</v>
+        <f>E19+9</f>
+        <v>44487</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="13">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
+      <c r="H19" s="13"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -3918,10 +3885,10 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18"/>
       <c r="B20" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="14">
         <v>1</v>
@@ -3931,13 +3898,13 @@
         <v>44478</v>
       </c>
       <c r="F20" s="29">
-        <f>E20+4</f>
-        <v>44482</v>
+        <f>E20+7</f>
+        <v>44485</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
@@ -3998,27 +3965,27 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18"/>
-      <c r="B21" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="35">
+      <c r="B21" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="14">
         <v>1</v>
       </c>
-      <c r="E21" s="36">
-        <f>E14+18</f>
-        <v>44488</v>
-      </c>
-      <c r="F21" s="36">
-        <f>E21</f>
-        <v>44488</v>
+      <c r="E21" s="29">
+        <f>F16+1</f>
+        <v>44478</v>
+      </c>
+      <c r="F21" s="29">
+        <f>E21+4</f>
+        <v>44482</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -4079,27 +4046,27 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18"/>
-      <c r="B22" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="14">
+      <c r="B22" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="35">
         <v>1</v>
       </c>
-      <c r="E22" s="29">
-        <f>F21</f>
+      <c r="E22" s="36">
+        <f>E14+18</f>
         <v>44488</v>
       </c>
-      <c r="F22" s="29">
-        <f>E22+6</f>
-        <v>44494</v>
+      <c r="F22" s="36">
+        <f>E22</f>
+        <v>44488</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -4161,26 +4128,26 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="18"/>
       <c r="B23" s="24" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D23" s="14">
         <v>1</v>
       </c>
       <c r="E23" s="29">
-        <f>E22+1</f>
-        <v>44489</v>
+        <f>F22</f>
+        <v>44488</v>
       </c>
       <c r="F23" s="29">
-        <f>E23+11</f>
-        <v>44500</v>
+        <f>E23+6</f>
+        <v>44494</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -4242,26 +4209,26 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="18"/>
       <c r="B24" s="24" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
       </c>
       <c r="E24" s="29">
-        <f>E22+1</f>
+        <f>E23+1</f>
         <v>44489</v>
       </c>
       <c r="F24" s="29">
-        <f>E24+15</f>
-        <v>44504</v>
+        <f>E24+11</f>
+        <v>44500</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -4323,16 +4290,16 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="18"/>
       <c r="B25" s="24" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D25" s="14">
         <v>1</v>
       </c>
       <c r="E25" s="29">
-        <f>E22+1</f>
+        <f>E23+1</f>
         <v>44489</v>
       </c>
       <c r="F25" s="29">
@@ -4403,25 +4370,28 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="18"/>
-      <c r="B26" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="35">
+      <c r="B26" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="14">
         <v>1</v>
       </c>
-      <c r="E26" s="36">
-        <f>F25+1</f>
-        <v>44505</v>
-      </c>
-      <c r="F26" s="36">
-        <f>E26</f>
-        <v>44505</v>
+      <c r="E26" s="29">
+        <f>E23+1</f>
+        <v>44489</v>
+      </c>
+      <c r="F26" s="29">
+        <f>E26+15</f>
+        <v>44504</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="13">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
@@ -4480,21 +4450,26 @@
       <c r="BL26" s="15"/>
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="35">
+        <v>1</v>
+      </c>
+      <c r="E27" s="36">
+        <f>F26+1</f>
+        <v>44505</v>
+      </c>
+      <c r="F27" s="36">
+        <f>E27</f>
+        <v>44505</v>
+      </c>
       <c r="G27" s="13"/>
-      <c r="H27" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H27" s="13"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
@@ -4553,28 +4528,20 @@
       <c r="BL27" s="15"/>
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="18"/>
-      <c r="B28" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="14">
-        <v>1</v>
-      </c>
-      <c r="E28" s="29">
-        <f>F26</f>
-        <v>44505</v>
-      </c>
-      <c r="F28" s="29">
-        <f>E28+3</f>
-        <v>44508</v>
-      </c>
+      <c r="A28" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="13">
+      <c r="H28" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -4636,26 +4603,26 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18"/>
       <c r="B29" s="24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D29" s="14">
         <v>1</v>
       </c>
       <c r="E29" s="29">
-        <f>E28+1</f>
-        <v>44506</v>
+        <f>F27</f>
+        <v>44505</v>
       </c>
       <c r="F29" s="29">
-        <f>E29+2</f>
+        <f>E29+3</f>
         <v>44508</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -4717,26 +4684,26 @@
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18"/>
       <c r="B30" s="24" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D30" s="14">
         <v>1</v>
       </c>
       <c r="E30" s="29">
-        <f>F29</f>
+        <f>E29+1</f>
+        <v>44506</v>
+      </c>
+      <c r="F30" s="29">
+        <f>E30+2</f>
         <v>44508</v>
-      </c>
-      <c r="F30" s="29">
-        <f>E30+6</f>
-        <v>44514</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -4798,7 +4765,7 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="18"/>
       <c r="B31" s="24" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>31</v>
@@ -4807,17 +4774,17 @@
         <v>1</v>
       </c>
       <c r="E31" s="29">
-        <f>F30+1</f>
-        <v>44515</v>
+        <f>F30</f>
+        <v>44508</v>
       </c>
       <c r="F31" s="29">
-        <f>E31+9</f>
-        <v>44524</v>
+        <f>E31+6</f>
+        <v>44514</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -4879,26 +4846,26 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18"/>
       <c r="B32" s="24" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D32" s="14">
         <v>1</v>
       </c>
       <c r="E32" s="29">
-        <f>F30+1</f>
+        <f>F31+1</f>
         <v>44515</v>
       </c>
       <c r="F32" s="29">
-        <f>E32+6</f>
-        <v>44521</v>
+        <f>E32+9</f>
+        <v>44524</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -4960,24 +4927,27 @@
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18"/>
       <c r="B33" s="24" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D33" s="14">
         <v>1</v>
       </c>
       <c r="E33" s="29">
-        <f>F30+1</f>
+        <f>F31+1</f>
         <v>44515</v>
       </c>
       <c r="F33" s="29">
-        <f>E33+10</f>
-        <v>44525</v>
+        <f>E33+6</f>
+        <v>44521</v>
       </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -5037,28 +5007,25 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="18"/>
-      <c r="B34" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="35">
+      <c r="B34" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="14">
         <v>1</v>
       </c>
-      <c r="E34" s="36">
-        <f>E26+21</f>
-        <v>44526</v>
-      </c>
-      <c r="F34" s="36">
-        <f>E34</f>
-        <v>44526</v>
+      <c r="E34" s="29">
+        <f>F31+1</f>
+        <v>44515</v>
+      </c>
+      <c r="F34" s="29">
+        <f>E34+10</f>
+        <v>44525</v>
       </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H34" s="13"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -5117,20 +5084,28 @@
       <c r="BL34" s="15"/>
     </row>
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="36">
+        <f>E27+21</f>
+        <v>44526</v>
+      </c>
+      <c r="F35" s="36">
+        <f>E35</f>
+        <v>44526</v>
+      </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="13" t="str">
+      <c r="H35" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -5190,28 +5165,20 @@
       <c r="BL35" s="15"/>
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1</v>
-      </c>
-      <c r="E36" s="29">
-        <f>F34+1</f>
-        <v>44527</v>
-      </c>
-      <c r="F36" s="29">
-        <f>E36+2</f>
-        <v>44529</v>
-      </c>
+      <c r="A36" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="13">
+      <c r="H36" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
@@ -5273,26 +5240,26 @@
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="24" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D37" s="14">
         <v>1</v>
       </c>
       <c r="E37" s="29">
-        <f>E36+1</f>
-        <v>44528</v>
+        <f>F35+1</f>
+        <v>44527</v>
       </c>
       <c r="F37" s="29">
-        <f>E40-1</f>
-        <v>44546</v>
+        <f>E37+2</f>
+        <v>44529</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
@@ -5354,20 +5321,20 @@
     <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="18"/>
       <c r="B38" s="24" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D38" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E38" s="29">
-        <f>E37</f>
+        <f>E37+1</f>
         <v>44528</v>
       </c>
       <c r="F38" s="29">
-        <f>F37</f>
+        <f>E41-1</f>
         <v>44546</v>
       </c>
       <c r="G38" s="13"/>
@@ -5435,13 +5402,13 @@
     <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="18"/>
       <c r="B39" s="24" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="D39" s="14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E39" s="29">
         <f>E38</f>
@@ -5452,7 +5419,10 @@
         <v>44546</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="H39" s="13">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
@@ -5512,28 +5482,25 @@
     </row>
     <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="18"/>
-      <c r="B40" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="35">
+      <c r="B40" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="14">
         <v>1</v>
       </c>
-      <c r="E40" s="36">
-        <f>E34+21</f>
-        <v>44547</v>
-      </c>
-      <c r="F40" s="36">
-        <f>E40</f>
-        <v>44547</v>
+      <c r="E40" s="29">
+        <f>E39</f>
+        <v>44528</v>
+      </c>
+      <c r="F40" s="29">
+        <f>F39</f>
+        <v>44546</v>
       </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H40" s="13"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
@@ -5592,20 +5559,28 @@
       <c r="BL40" s="15"/>
     </row>
     <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="35">
+        <v>1</v>
+      </c>
+      <c r="E41" s="36">
+        <f>E35+21</f>
+        <v>44547</v>
+      </c>
+      <c r="F41" s="36">
+        <f>E41</f>
+        <v>44547</v>
+      </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="13" t="str">
+      <c r="H41" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -5665,28 +5640,20 @@
       <c r="BL41" s="15"/>
     </row>
     <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="18"/>
-      <c r="B42" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="14">
-        <v>1</v>
-      </c>
-      <c r="E42" s="29">
-        <f>E40</f>
-        <v>44547</v>
-      </c>
-      <c r="F42" s="29">
-        <f>E42+1</f>
-        <v>44548</v>
-      </c>
+      <c r="A42" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="38"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="13">
+      <c r="H42" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -5747,27 +5714,27 @@
     </row>
     <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="18"/>
-      <c r="B43" s="32" t="s">
-        <v>60</v>
+      <c r="B43" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" s="14">
         <v>1</v>
       </c>
       <c r="E43" s="29">
-        <f>F42+1</f>
-        <v>44549</v>
+        <f>E41</f>
+        <v>44547</v>
       </c>
       <c r="F43" s="29">
-        <f>E43+7</f>
-        <v>44556</v>
+        <f>E43+1</f>
+        <v>44548</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -5828,27 +5795,27 @@
     </row>
     <row r="44" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="18"/>
-      <c r="B44" s="24" t="s">
-        <v>67</v>
+      <c r="B44" s="32" t="s">
+        <v>55</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D44" s="14">
         <v>1</v>
       </c>
       <c r="E44" s="29">
-        <f>F43</f>
+        <f>F43+1</f>
+        <v>44549</v>
+      </c>
+      <c r="F44" s="29">
+        <f>E44+7</f>
         <v>44556</v>
-      </c>
-      <c r="F44" s="29">
-        <f>E46-1</f>
-        <v>44585</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
@@ -5910,26 +5877,26 @@
     <row r="45" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="18"/>
       <c r="B45" s="24" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="D45" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E45" s="29">
-        <f>F42+1</f>
-        <v>44549</v>
+        <f>F44</f>
+        <v>44556</v>
       </c>
       <c r="F45" s="29">
-        <f>E46-1</f>
+        <f>E47-1</f>
         <v>44585</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
@@ -5990,27 +5957,27 @@
     </row>
     <row r="46" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="18"/>
-      <c r="B46" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="35">
-        <v>1</v>
-      </c>
-      <c r="E46" s="36">
-        <f>E40+39</f>
-        <v>44586</v>
-      </c>
-      <c r="F46" s="36">
-        <f>E46</f>
-        <v>44586</v>
+      <c r="B46" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="E46" s="29">
+        <f>F43+1</f>
+        <v>44549</v>
+      </c>
+      <c r="F46" s="29">
+        <f>E47-1</f>
+        <v>44585</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
@@ -6070,20 +6037,28 @@
       <c r="BL46" s="15"/>
     </row>
     <row r="47" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="38"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="35">
+        <v>1</v>
+      </c>
+      <c r="E47" s="36">
+        <f>E41+39</f>
+        <v>44586</v>
+      </c>
+      <c r="F47" s="36">
+        <f>E47</f>
+        <v>44586</v>
+      </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="13" t="str">
+      <c r="H47" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -6143,26 +6118,20 @@
       <c r="BL47" s="15"/>
     </row>
     <row r="48" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="18"/>
-      <c r="B48" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="14">
-        <v>1</v>
-      </c>
-      <c r="E48" s="29">
-        <f>F46+1</f>
-        <v>44587</v>
-      </c>
-      <c r="F48" s="29">
-        <f>E48</f>
-        <v>44587</v>
-      </c>
+      <c r="A48" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="38"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
       <c r="G48" s="13"/>
-      <c r="H48" s="13">
+      <c r="H48" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
@@ -6224,26 +6193,24 @@
     <row r="49" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="18"/>
       <c r="B49" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>29</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C49" s="22"/>
       <c r="D49" s="14">
         <v>1</v>
       </c>
       <c r="E49" s="29">
-        <f>F48+1</f>
-        <v>44588</v>
+        <f>F47+1</f>
+        <v>44587</v>
       </c>
       <c r="F49" s="29">
-        <f>E49+7</f>
-        <v>44595</v>
+        <f>E49</f>
+        <v>44587</v>
       </c>
       <c r="G49" s="13"/>
       <c r="H49" s="13">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
@@ -6305,24 +6272,27 @@
     <row r="50" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="18"/>
       <c r="B50" s="24" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D50" s="14">
         <v>1</v>
       </c>
       <c r="E50" s="29">
         <f>F49+1</f>
-        <v>44596</v>
+        <v>44588</v>
       </c>
       <c r="F50" s="29">
-        <f>E50+21</f>
-        <v>44617</v>
+        <f>E50+7</f>
+        <v>44595</v>
       </c>
       <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
+      <c r="H50" s="13">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -6383,20 +6353,20 @@
     <row r="51" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="18"/>
       <c r="B51" s="24" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D51" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E51" s="29">
-        <f>E50</f>
+        <f>F50+1</f>
         <v>44596</v>
       </c>
       <c r="F51" s="29">
-        <f>F50</f>
+        <f>E51+21</f>
         <v>44617</v>
       </c>
       <c r="G51" s="13"/>
@@ -6461,13 +6431,13 @@
     <row r="52" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="18"/>
       <c r="B52" s="24" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D52" s="14">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E52" s="29">
         <f>E51</f>
@@ -6539,20 +6509,20 @@
     <row r="53" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="18"/>
       <c r="B53" s="24" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="D53" s="14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E53" s="29">
-        <f>F49+1</f>
+        <f>E52</f>
         <v>44596</v>
       </c>
       <c r="F53" s="29">
-        <f>E53+21</f>
+        <f>F52</f>
         <v>44617</v>
       </c>
       <c r="G53" s="13"/>
@@ -6617,21 +6587,21 @@
     <row r="54" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="18"/>
       <c r="B54" s="24" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D54" s="14">
         <v>1</v>
       </c>
       <c r="E54" s="29">
-        <f>F53+1</f>
-        <v>44618</v>
+        <f>F50+1</f>
+        <v>44596</v>
       </c>
       <c r="F54" s="29">
-        <f>E54+4</f>
-        <v>44622</v>
+        <f>E54+21</f>
+        <v>44617</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
@@ -6694,28 +6664,25 @@
     </row>
     <row r="55" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="18"/>
-      <c r="B55" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D55" s="35">
+      <c r="B55" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="14">
         <v>1</v>
       </c>
-      <c r="E55" s="36">
-        <f>F46+37</f>
-        <v>44623</v>
-      </c>
-      <c r="F55" s="36">
-        <f>E55</f>
-        <v>44623</v>
+      <c r="E55" s="29">
+        <f>F54+1</f>
+        <v>44618</v>
+      </c>
+      <c r="F55" s="29">
+        <f>E55+4</f>
+        <v>44622</v>
       </c>
       <c r="G55" s="13"/>
-      <c r="H55" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H55" s="13"/>
       <c r="I55" s="15"/>
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
@@ -6774,20 +6741,28 @@
       <c r="BL55" s="15"/>
     </row>
     <row r="56" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" s="38"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="35">
+        <v>1</v>
+      </c>
+      <c r="E56" s="36">
+        <f>F47+37</f>
+        <v>44623</v>
+      </c>
+      <c r="F56" s="36">
+        <f>E56</f>
+        <v>44623</v>
+      </c>
       <c r="G56" s="13"/>
-      <c r="H56" s="13" t="str">
+      <c r="H56" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
@@ -6847,26 +6822,20 @@
       <c r="BL56" s="15"/>
     </row>
     <row r="57" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="18"/>
-      <c r="B57" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D57" s="14">
-        <v>1</v>
-      </c>
-      <c r="E57" s="29">
-        <v>44624</v>
-      </c>
-      <c r="F57" s="29">
-        <v>44624</v>
-      </c>
+      <c r="A57" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="38"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
       <c r="G57" s="13"/>
-      <c r="H57" s="13">
+      <c r="H57" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
@@ -6928,24 +6897,24 @@
     <row r="58" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="18"/>
       <c r="B58" s="24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="D58" s="14">
         <v>1</v>
       </c>
       <c r="E58" s="29">
-        <v>44625</v>
+        <v>44624</v>
       </c>
       <c r="F58" s="29">
-        <v>44631</v>
+        <v>44624</v>
       </c>
       <c r="G58" s="13"/>
       <c r="H58" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
@@ -7007,22 +6976,25 @@
     <row r="59" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="18"/>
       <c r="B59" s="24" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D59" s="14">
         <v>1</v>
       </c>
       <c r="E59" s="29">
-        <v>44632</v>
+        <v>44625</v>
       </c>
       <c r="F59" s="29">
-        <v>44645</v>
+        <v>44631</v>
       </c>
       <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
+      <c r="H59" s="13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
@@ -7083,10 +7055,10 @@
     <row r="60" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="18"/>
       <c r="B60" s="24" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="D60" s="14">
         <v>1</v>
@@ -7159,10 +7131,10 @@
     <row r="61" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="18"/>
       <c r="B61" s="24" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="D61" s="14">
         <v>1</v>
@@ -7235,10 +7207,10 @@
     <row r="62" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="18"/>
       <c r="B62" s="24" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="D62" s="14">
         <v>1</v>
@@ -7250,10 +7222,7 @@
         <v>44645</v>
       </c>
       <c r="G62" s="13"/>
-      <c r="H62" s="13">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
+      <c r="H62" s="13"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
@@ -7312,20 +7281,26 @@
       <c r="BL62" s="15"/>
     </row>
     <row r="63" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C63" s="38"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="E63" s="29">
+        <v>44632</v>
+      </c>
+      <c r="F63" s="29">
+        <v>44645</v>
+      </c>
       <c r="G63" s="13"/>
-      <c r="H63" s="13" t="str">
+      <c r="H63" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
@@ -7387,25 +7362,22 @@
     <row r="64" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="18"/>
       <c r="B64" s="24" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="D64" s="14">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E64" s="29">
-        <v>44646</v>
+        <v>44632</v>
       </c>
       <c r="F64" s="29">
-        <v>44653</v>
+        <v>44645</v>
       </c>
       <c r="G64" s="13"/>
-      <c r="H64" s="13">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
+      <c r="H64" s="13"/>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
       <c r="K64" s="15"/>
@@ -7464,12 +7436,16 @@
       <c r="BL64" s="15"/>
     </row>
     <row r="65" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="18"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="A65" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="38"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13" t="str">
         <f t="shared" si="4"/>
@@ -7534,26 +7510,25 @@
     </row>
     <row r="66" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="18"/>
-      <c r="B66" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" s="35">
+      <c r="B66" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="14">
         <v>0</v>
       </c>
-      <c r="E66" s="36">
-        <v>44655</v>
-      </c>
-      <c r="F66" s="36">
-        <f>E66+12</f>
-        <v>44667</v>
+      <c r="E66" s="29">
+        <v>44646</v>
+      </c>
+      <c r="F66" s="29">
+        <v>44653</v>
       </c>
       <c r="G66" s="13"/>
       <c r="H66" s="13">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
@@ -7613,16 +7588,12 @@
       <c r="BL66" s="15"/>
     </row>
     <row r="67" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="38"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
+      <c r="A67" s="18"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13" t="str">
         <f t="shared" si="4"/>
@@ -7687,19 +7658,26 @@
     </row>
     <row r="68" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="18"/>
-      <c r="B68" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="14">
+      <c r="B68" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="35">
         <v>0</v>
       </c>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
+      <c r="E68" s="36">
+        <v>44655</v>
+      </c>
+      <c r="F68" s="36">
+        <f>E68+12</f>
+        <v>44667</v>
+      </c>
       <c r="G68" s="13"/>
-      <c r="H68" s="13" t="str">
+      <c r="H68" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
@@ -7759,18 +7737,16 @@
       <c r="BL68" s="15"/>
     </row>
     <row r="69" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="18"/>
-      <c r="B69" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="14">
-        <v>0</v>
-      </c>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
+      <c r="A69" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="38"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13" t="str">
         <f t="shared" si="4"/>
@@ -7835,9 +7811,13 @@
     </row>
     <row r="70" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="18"/>
-      <c r="B70" s="24"/>
+      <c r="B70" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="C70" s="22"/>
-      <c r="D70" s="14"/>
+      <c r="D70" s="14">
+        <v>0</v>
+      </c>
       <c r="E70" s="29"/>
       <c r="F70" s="29"/>
       <c r="G70" s="13"/>
@@ -7904,27 +7884,21 @@
     </row>
     <row r="71" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="18"/>
-      <c r="B71" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" s="35">
+      <c r="B71" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="14">
         <v>0</v>
       </c>
-      <c r="E71" s="36">
-        <f>E66+35</f>
-        <v>44690</v>
-      </c>
-      <c r="F71" s="36">
-        <f>E71+12</f>
-        <v>44702</v>
-      </c>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
       <c r="G71" s="13"/>
-      <c r="H71" s="13">
+      <c r="H71" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v/>
       </c>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
@@ -7984,16 +7958,12 @@
       <c r="BL71" s="15"/>
     </row>
     <row r="72" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="40"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13" t="str">
         <f t="shared" si="4"/>
@@ -8058,19 +8028,27 @@
     </row>
     <row r="73" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="18"/>
-      <c r="B73" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="14">
+      <c r="B73" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="35">
         <v>0</v>
       </c>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
+      <c r="E73" s="36">
+        <f>E68+35</f>
+        <v>44690</v>
+      </c>
+      <c r="F73" s="36">
+        <f>E73+12</f>
+        <v>44702</v>
+      </c>
       <c r="G73" s="13"/>
-      <c r="H73" s="13" t="str">
+      <c r="H73" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
@@ -8130,18 +8108,16 @@
       <c r="BL73" s="15"/>
     </row>
     <row r="74" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="18"/>
-      <c r="B74" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D74" s="14">
-        <v>0</v>
-      </c>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
+      <c r="A74" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="38"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="40"/>
+      <c r="F74" s="40"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13" t="str">
         <f t="shared" si="4"/>
@@ -8206,9 +8182,13 @@
     </row>
     <row r="75" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="18"/>
-      <c r="B75" s="24"/>
+      <c r="B75" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="C75" s="22"/>
-      <c r="D75" s="14"/>
+      <c r="D75" s="14">
+        <v>0</v>
+      </c>
       <c r="E75" s="29"/>
       <c r="F75" s="29"/>
       <c r="G75" s="13"/>
@@ -8275,25 +8255,21 @@
     </row>
     <row r="76" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="18"/>
-      <c r="B76" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D76" s="35"/>
-      <c r="E76" s="36">
-        <f>E71+5</f>
-        <v>44695</v>
-      </c>
-      <c r="F76" s="36">
-        <f>E76</f>
-        <v>44695</v>
-      </c>
+      <c r="B76" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="14">
+        <v>0</v>
+      </c>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
       <c r="G76" s="13"/>
-      <c r="H76" s="13">
+      <c r="H76" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I76" s="15"/>
       <c r="J76" s="15"/>
@@ -8353,14 +8329,12 @@
       <c r="BL76" s="15"/>
     </row>
     <row r="77" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13" t="str">
         <f t="shared" si="4"/>
@@ -8423,23 +8397,168 @@
       <c r="BK77" s="15"/>
       <c r="BL77" s="15"/>
     </row>
-    <row r="78" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G78" s="6"/>
+    <row r="78" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="18"/>
+      <c r="B78" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" s="35"/>
+      <c r="E78" s="36">
+        <f>E73+5</f>
+        <v>44695</v>
+      </c>
+      <c r="F78" s="36">
+        <f>E78</f>
+        <v>44695</v>
+      </c>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
+      <c r="AM78" s="15"/>
+      <c r="AN78" s="15"/>
+      <c r="AO78" s="15"/>
+      <c r="AP78" s="15"/>
+      <c r="AQ78" s="15"/>
+      <c r="AR78" s="15"/>
+      <c r="AS78" s="15"/>
+      <c r="AT78" s="15"/>
+      <c r="AU78" s="15"/>
+      <c r="AV78" s="15"/>
+      <c r="AW78" s="15"/>
+      <c r="AX78" s="15"/>
+      <c r="AY78" s="15"/>
+      <c r="AZ78" s="15"/>
+      <c r="BA78" s="15"/>
+      <c r="BB78" s="15"/>
+      <c r="BC78" s="15"/>
+      <c r="BD78" s="15"/>
+      <c r="BE78" s="15"/>
+      <c r="BF78" s="15"/>
+      <c r="BG78" s="15"/>
+      <c r="BH78" s="15"/>
+      <c r="BI78" s="15"/>
+      <c r="BJ78" s="15"/>
+      <c r="BK78" s="15"/>
+      <c r="BL78" s="15"/>
     </row>
-    <row r="79" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="10"/>
-      <c r="F79" s="20"/>
+    <row r="79" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="25"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+      <c r="AB79" s="15"/>
+      <c r="AC79" s="15"/>
+      <c r="AD79" s="15"/>
+      <c r="AE79" s="15"/>
+      <c r="AF79" s="15"/>
+      <c r="AG79" s="15"/>
+      <c r="AH79" s="15"/>
+      <c r="AI79" s="15"/>
+      <c r="AJ79" s="15"/>
+      <c r="AK79" s="15"/>
+      <c r="AL79" s="15"/>
+      <c r="AM79" s="15"/>
+      <c r="AN79" s="15"/>
+      <c r="AO79" s="15"/>
+      <c r="AP79" s="15"/>
+      <c r="AQ79" s="15"/>
+      <c r="AR79" s="15"/>
+      <c r="AS79" s="15"/>
+      <c r="AT79" s="15"/>
+      <c r="AU79" s="15"/>
+      <c r="AV79" s="15"/>
+      <c r="AW79" s="15"/>
+      <c r="AX79" s="15"/>
+      <c r="AY79" s="15"/>
+      <c r="AZ79" s="15"/>
+      <c r="BA79" s="15"/>
+      <c r="BB79" s="15"/>
+      <c r="BC79" s="15"/>
+      <c r="BD79" s="15"/>
+      <c r="BE79" s="15"/>
+      <c r="BF79" s="15"/>
+      <c r="BG79" s="15"/>
+      <c r="BH79" s="15"/>
+      <c r="BI79" s="15"/>
+      <c r="BJ79" s="15"/>
+      <c r="BK79" s="15"/>
+      <c r="BL79" s="15"/>
     </row>
     <row r="80" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="11"/>
+      <c r="G80" s="6"/>
+    </row>
+    <row r="81" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="10"/>
+      <c r="F81" s="20"/>
+    </row>
+    <row r="82" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C82" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="W5:AC5"/>
-    <mergeCell ref="AD5:AJ5"/>
-    <mergeCell ref="AK5:AQ5"/>
-    <mergeCell ref="AR5:AX5"/>
     <mergeCell ref="AY5:BE5"/>
     <mergeCell ref="BF5:BL5"/>
     <mergeCell ref="B2:B4"/>
@@ -8448,8 +8567,13 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="I5:O5"/>
     <mergeCell ref="P5:V5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="W5:AC5"/>
+    <mergeCell ref="AD5:AJ5"/>
+    <mergeCell ref="AK5:AQ5"/>
+    <mergeCell ref="AR5:AX5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D15:D16 D77 D22:D25 D18:D20 D64:D65">
+  <conditionalFormatting sqref="D15:D16 D79 D23:D26 D18:D21 D66:D67 D49:D55">
     <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8463,20 +8587,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77:BL77 I32:BL34 I6:BL25 I27:BL29 I63:BL65">
-    <cfRule type="expression" dxfId="53" priority="124">
+  <conditionalFormatting sqref="I79:BL79 I33:BL35 I6:BL26 I28:BL30 I65:BL67 I48:BL55">
+    <cfRule type="expression" dxfId="50" priority="124">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77:BL77 I32:BL34 I8:BL25 I27:BL29 I63:BL65">
-    <cfRule type="expression" dxfId="52" priority="122">
+  <conditionalFormatting sqref="I79:BL79 I33:BL35 I8:BL26 I28:BL30 I65:BL67 I48:BL55">
+    <cfRule type="expression" dxfId="49" priority="122">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="123" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="123" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32:D33 D28:D29">
+  <conditionalFormatting sqref="D33:D34 D29:D30">
     <cfRule type="dataBar" priority="120">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8490,7 +8614,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8504,20 +8628,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41:BL43 I45:BL45">
-    <cfRule type="expression" dxfId="50" priority="119">
+  <conditionalFormatting sqref="I42:BL44 I46:BL46">
+    <cfRule type="expression" dxfId="47" priority="119">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41:BL43 I45:BL45">
-    <cfRule type="expression" dxfId="49" priority="117">
+  <conditionalFormatting sqref="I42:BL44 I46:BL46">
+    <cfRule type="expression" dxfId="46" priority="117">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="118" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:D43">
+  <conditionalFormatting sqref="D43:D44">
     <cfRule type="dataBar" priority="115">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8531,52 +8655,25 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46:BL46">
-    <cfRule type="expression" dxfId="47" priority="113">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="44" priority="113">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46:BL46">
-    <cfRule type="expression" dxfId="46" priority="111">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="43" priority="111">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="112" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL54">
-    <cfRule type="expression" dxfId="44" priority="110">
-      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL54">
-    <cfRule type="expression" dxfId="43" priority="108">
-      <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="109" stopIfTrue="1">
-      <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D54">
-    <cfRule type="dataBar" priority="106">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{29449E41-F591-4B88-A4DB-237D24C5C4C9}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I55:BL55">
+  <conditionalFormatting sqref="I56:BL56">
     <cfRule type="expression" dxfId="41" priority="104">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I55:BL55">
+  <conditionalFormatting sqref="I56:BL56">
     <cfRule type="expression" dxfId="40" priority="102">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8584,7 +8681,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
+  <conditionalFormatting sqref="D63:D64">
     <cfRule type="dataBar" priority="98">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8598,12 +8695,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL62">
+  <conditionalFormatting sqref="I57:BL64">
     <cfRule type="expression" dxfId="38" priority="101">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL62">
+  <conditionalFormatting sqref="I57:BL64">
     <cfRule type="expression" dxfId="37" priority="99">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8611,7 +8708,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57:D61">
+  <conditionalFormatting sqref="D58:D62">
     <cfRule type="dataBar" priority="97">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8653,7 +8750,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D72">
     <cfRule type="dataBar" priority="80">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8667,12 +8764,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67:BL70">
+  <conditionalFormatting sqref="I69:BL72">
     <cfRule type="expression" dxfId="35" priority="83">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67:BL70">
+  <conditionalFormatting sqref="I69:BL72">
     <cfRule type="expression" dxfId="34" priority="81">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8680,12 +8777,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66:BL66">
+  <conditionalFormatting sqref="I68:BL68">
     <cfRule type="expression" dxfId="32" priority="79">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66:BL66">
+  <conditionalFormatting sqref="I68:BL68">
     <cfRule type="expression" dxfId="31" priority="77">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8693,7 +8790,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68:D69">
+  <conditionalFormatting sqref="D70:D71">
     <cfRule type="dataBar" priority="75">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8707,7 +8804,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="D77">
     <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8721,12 +8818,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72:BL75">
+  <conditionalFormatting sqref="I74:BL77">
     <cfRule type="expression" dxfId="29" priority="73">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72:BL75">
+  <conditionalFormatting sqref="I74:BL77">
     <cfRule type="expression" dxfId="28" priority="71">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8734,12 +8831,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71:BL71">
+  <conditionalFormatting sqref="I73:BL73">
     <cfRule type="expression" dxfId="26" priority="69">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71:BL71">
+  <conditionalFormatting sqref="I73:BL73">
     <cfRule type="expression" dxfId="25" priority="67">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8747,7 +8844,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73:D74">
+  <conditionalFormatting sqref="D75:D76">
     <cfRule type="dataBar" priority="65">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8761,12 +8858,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76:BL76">
+  <conditionalFormatting sqref="I78:BL78">
     <cfRule type="expression" dxfId="23" priority="63">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76:BL76">
+  <conditionalFormatting sqref="I78:BL78">
     <cfRule type="expression" dxfId="22" priority="61">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8774,12 +8871,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:BL30">
+  <conditionalFormatting sqref="I31:BL31">
     <cfRule type="expression" dxfId="20" priority="59">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:BL30">
+  <conditionalFormatting sqref="I31:BL31">
     <cfRule type="expression" dxfId="19" priority="57">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8787,7 +8884,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="D31">
     <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8801,12 +8898,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:BL31">
+  <conditionalFormatting sqref="I32:BL32">
     <cfRule type="expression" dxfId="17" priority="55">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:BL31">
+  <conditionalFormatting sqref="I32:BL32">
     <cfRule type="expression" dxfId="16" priority="53">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8814,7 +8911,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8828,12 +8925,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:BL36 I40:BL40">
+  <conditionalFormatting sqref="I36:BL37 I41:BL41">
     <cfRule type="expression" dxfId="14" priority="51">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:BL36 I40:BL40">
+  <conditionalFormatting sqref="I36:BL37 I41:BL41">
     <cfRule type="expression" dxfId="13" priority="49">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8841,7 +8938,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="dataBar" priority="48">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8855,12 +8952,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:BL37">
+  <conditionalFormatting sqref="I38:BL38">
     <cfRule type="expression" dxfId="11" priority="47">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:BL37">
+  <conditionalFormatting sqref="I38:BL38">
     <cfRule type="expression" dxfId="10" priority="45">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8868,7 +8965,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D38">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8882,12 +8979,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL39">
+  <conditionalFormatting sqref="I39:BL40">
     <cfRule type="expression" dxfId="8" priority="43">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL39">
+  <conditionalFormatting sqref="I39:BL40">
     <cfRule type="expression" dxfId="7" priority="41">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8895,7 +8992,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
+  <conditionalFormatting sqref="D39:D40">
     <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8909,7 +9006,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D45">
     <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8923,12 +9020,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:BL44">
+  <conditionalFormatting sqref="I45:BL45">
     <cfRule type="expression" dxfId="5" priority="39">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:BL44">
+  <conditionalFormatting sqref="I45:BL45">
     <cfRule type="expression" dxfId="4" priority="37">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8992,7 +9089,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D22">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9006,7 +9103,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9020,7 +9117,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
+  <conditionalFormatting sqref="D41">
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9034,7 +9131,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9048,7 +9145,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9062,7 +9159,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D68">
     <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9076,7 +9173,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
+  <conditionalFormatting sqref="D73">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9090,7 +9187,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D76">
+  <conditionalFormatting sqref="D78">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9104,7 +9201,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
+  <conditionalFormatting sqref="D28">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9118,7 +9215,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9132,7 +9229,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9146,7 +9243,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9160,7 +9257,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9174,7 +9271,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
+  <conditionalFormatting sqref="D65">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9188,7 +9285,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
+  <conditionalFormatting sqref="D69">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9202,7 +9299,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
+  <conditionalFormatting sqref="D74">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9216,12 +9313,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:BL26">
+  <conditionalFormatting sqref="I27:BL27">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:BL26">
+  <conditionalFormatting sqref="I27:BL27">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -9229,7 +9326,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="D27">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9270,7 +9367,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15:D16 D77 D22:D25 D18:D20 D64:D65</xm:sqref>
+          <xm:sqref>D15:D16 D79 D23:D26 D18:D21 D66:D67 D49:D55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{61BAFCB1-C9D1-4453-9835-894AAFFB2D48}">
@@ -9285,7 +9382,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D32:D33 D28:D29</xm:sqref>
+          <xm:sqref>D33:D34 D29:D30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AD57E977-98C8-4463-AF63-0B910B22A855}">
@@ -9300,7 +9397,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D45</xm:sqref>
+          <xm:sqref>D46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{85DD6914-E53C-41B0-AFBA-86F7B9451DA6}">
@@ -9315,22 +9412,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D42:D43</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{29449E41-F591-4B88-A4DB-237D24C5C4C9}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D48:D54</xm:sqref>
+          <xm:sqref>D43:D44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F7F63C90-679F-41E1-9DD7-C7641723B832}">
@@ -9345,7 +9427,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D62</xm:sqref>
+          <xm:sqref>D63:D64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8C1F1D87-2F5D-4508-9015-0F4807608336}">
@@ -9360,7 +9442,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D57:D61</xm:sqref>
+          <xm:sqref>D58:D62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{85676472-4DEA-4B47-8076-2B079F7EB722}">
@@ -9405,7 +9487,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D70</xm:sqref>
+          <xm:sqref>D72</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D92EFAD8-9A39-41D6-8E74-09FCB7C99446}">
@@ -9420,7 +9502,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D68:D69</xm:sqref>
+          <xm:sqref>D70:D71</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{49690BEA-F1DA-49A9-87E0-BC10D33392B4}">
@@ -9435,7 +9517,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D75</xm:sqref>
+          <xm:sqref>D77</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F3BCBE8B-1131-4EC4-93C6-93A3D2241A3A}">
@@ -9450,7 +9532,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D73:D74</xm:sqref>
+          <xm:sqref>D75:D76</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{70FE4911-65CD-4B63-902B-DAD573D9D1E7}">
@@ -9465,7 +9547,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D30</xm:sqref>
+          <xm:sqref>D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{107B3D2A-9D99-4B77-A0C1-E7D4234EC328}">
@@ -9480,7 +9562,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D31</xm:sqref>
+          <xm:sqref>D32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4BDF0497-329E-4ACE-A091-C6666647B0A6}">
@@ -9495,7 +9577,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36</xm:sqref>
+          <xm:sqref>D37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2616EACB-B142-4ABA-AB98-D0EFAE3192B1}">
@@ -9510,7 +9592,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D37</xm:sqref>
+          <xm:sqref>D38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9179826B-45ED-4988-BB2A-78DA7424E602}">
@@ -9525,7 +9607,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D38:D39</xm:sqref>
+          <xm:sqref>D39:D40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9795FCF7-A67A-433E-B155-AD1C0E7C374A}">
@@ -9540,7 +9622,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D44</xm:sqref>
+          <xm:sqref>D45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{36C8D48B-9FF9-4463-BC3F-14FABEE2DEF7}">
@@ -9615,7 +9697,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D21</xm:sqref>
+          <xm:sqref>D22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DE1AD479-0A37-44F4-AC20-51FF297665D3}">
@@ -9630,7 +9712,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{49FBE34D-D83B-497D-AB99-28B0686734FB}">
@@ -9645,7 +9727,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D40</xm:sqref>
+          <xm:sqref>D41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FFA7516B-0875-4D87-99ED-B7E4CACCC0E1}">
@@ -9660,7 +9742,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D46</xm:sqref>
+          <xm:sqref>D47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{66BA6DFA-1489-4D78-8D16-D0BABA15730F}">
@@ -9675,7 +9757,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D55</xm:sqref>
+          <xm:sqref>D56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F9FF2D8E-4C48-4314-AE00-D91E4BEBF00D}">
@@ -9690,7 +9772,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D66</xm:sqref>
+          <xm:sqref>D68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{47FD5541-751B-48F2-895B-231260031964}">
@@ -9705,7 +9787,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D71</xm:sqref>
+          <xm:sqref>D73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CB458C94-EC1D-48A0-8F37-BA38EE604418}">
@@ -9720,7 +9802,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D76</xm:sqref>
+          <xm:sqref>D78</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AC19E591-9826-41D2-8753-21A5AEC1982F}">
@@ -9735,7 +9817,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D27</xm:sqref>
+          <xm:sqref>D28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7E87486C-C83F-46B9-BB58-D6A8CEED9048}">
@@ -9750,7 +9832,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1FF748D9-3BCB-4034-9208-1F2D65C79F13}">
@@ -9765,7 +9847,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D41</xm:sqref>
+          <xm:sqref>D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F2C994C7-19E2-44FD-954A-AB7D6DE46441}">
@@ -9780,7 +9862,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D47</xm:sqref>
+          <xm:sqref>D48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8CA27610-5A3B-4302-BEA5-774F42E0EC59}">
@@ -9795,7 +9877,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D56</xm:sqref>
+          <xm:sqref>D57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B566DAE9-59F0-494F-B4A5-6CA202ED05AF}">
@@ -9810,7 +9892,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D63</xm:sqref>
+          <xm:sqref>D65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E8B7A00D-0A45-4E39-935E-0EF6E104B91A}">
@@ -9825,7 +9907,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D67</xm:sqref>
+          <xm:sqref>D69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{61C46EA8-F9E7-45B9-92F2-CA890223D6D5}">
@@ -9840,7 +9922,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D72</xm:sqref>
+          <xm:sqref>D74</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8A618AE5-6A10-402E-8877-7F8471EF9C36}">
@@ -9855,7 +9937,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D26</xm:sqref>
+          <xm:sqref>D27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Mise à jour sprint 7 et 8 dans planning
</commit_message>
<xml_diff>
--- a/Documents/0_Planning.xlsx
+++ b/Documents/0_Planning.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D28C6C7-427A-4BEE-86B1-591F50367233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E434DCB-B18E-4498-8F7E-2D461C7C4D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="3444" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningProjet" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Réunion Point de contrôle (A2.1)</t>
-  </si>
-  <si>
-    <t>Révision des points abordés en Point de contrôle (A3.2)</t>
   </si>
   <si>
     <t>Réunion A4</t>
@@ -354,9 +351,6 @@
     <t>Modélisation de l'application de WavCom</t>
   </si>
   <si>
-    <t>Document étude d'opportunité et liste des risques</t>
-  </si>
-  <si>
     <t>Révision de l'étude d'opportunité et de la liste des risques</t>
   </si>
   <si>
@@ -397,6 +391,45 @@
   </si>
   <si>
     <t>Documentation des jeux de tests</t>
+  </si>
+  <si>
+    <t>Document utilisation WavMap</t>
+  </si>
+  <si>
+    <t>Améliorer performance API</t>
+  </si>
+  <si>
+    <t>Créer le backEnd partie WavMap</t>
+  </si>
+  <si>
+    <t>Lier la base de données à WavMap</t>
+  </si>
+  <si>
+    <t>Jeux de tests sécurité et performance</t>
+  </si>
+  <si>
+    <t>Créer le frontEnd partie WavMap</t>
+  </si>
+  <si>
+    <t>Connecter la base de données WavCom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonctionnalité réserver le matériel </t>
+  </si>
+  <si>
+    <t>Fonctionnalité chat WavCom</t>
+  </si>
+  <si>
+    <t>Vérifier toutes les fonctionnalités WavCom</t>
+  </si>
+  <si>
+    <t>Liaison calendrier disponibiltés Waview avec leur calendrier personnel</t>
+  </si>
+  <si>
+    <t>Création liste des risques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document étude d'opportunité </t>
   </si>
 </sst>
 </file>
@@ -2281,27 +2314,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL82"/>
+  <dimension ref="A1:BL92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="7" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.453125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="53.81640625" customWidth="1"/>
-    <col min="3" max="3" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.453125" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2315,7 +2348,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="19"/>
       <c r="B2" s="45" t="s">
         <v>29</v>
@@ -2327,7 +2360,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="19"/>
       <c r="B3" s="45"/>
       <c r="C3" s="1"/>
@@ -2337,7 +2370,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:64" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
@@ -2351,7 +2384,7 @@
       </c>
       <c r="F4" s="48"/>
     </row>
-    <row r="5" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
@@ -2443,7 +2476,7 @@
       <c r="BK5" s="43"/>
       <c r="BL5" s="44"/>
     </row>
-    <row r="6" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
@@ -2678,7 +2711,7 @@
         <v>44668</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
@@ -2926,12 +2959,12 @@
         <v>d</v>
       </c>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
@@ -2939,7 +2972,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H79" si="4">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
+        <f t="shared" ref="H8:H89" si="4">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
         <v/>
       </c>
       <c r="I8" s="15"/>
@@ -2999,7 +3032,7 @@
       <c r="BK8" s="15"/>
       <c r="BL8" s="15"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
@@ -3081,7 +3114,7 @@
       <c r="BK9" s="15"/>
       <c r="BL9" s="15"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
@@ -3164,7 +3197,7 @@
       <c r="BK10" s="15"/>
       <c r="BL10" s="15"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="24" t="s">
         <v>21</v>
@@ -3245,10 +3278,10 @@
       <c r="BK11" s="15"/>
       <c r="BL11" s="15"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="24" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>26</v>
@@ -3326,30 +3359,25 @@
       <c r="BK12" s="15"/>
       <c r="BL12" s="15"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="18"/>
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
       <c r="B13" s="24" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="D13" s="14">
         <v>1</v>
       </c>
       <c r="E13" s="29">
-        <f>F10+1</f>
-        <v>44466</v>
+        <v>44463</v>
       </c>
       <c r="F13" s="29">
-        <f>E13+3</f>
-        <v>44469</v>
+        <v>44465</v>
       </c>
       <c r="G13" s="13"/>
-      <c r="H13" s="13">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
+      <c r="H13" s="13"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -3362,8 +3390,8 @@
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
       <c r="W13" s="15"/>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
@@ -3407,29 +3435,29 @@
       <c r="BK13" s="15"/>
       <c r="BL13" s="15"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18"/>
-      <c r="B14" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="35">
+      <c r="B14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="14">
         <v>1</v>
       </c>
-      <c r="E14" s="36">
-        <f>F13+1</f>
-        <v>44470</v>
-      </c>
-      <c r="F14" s="36">
-        <f>E14</f>
-        <v>44470</v>
+      <c r="E14" s="29">
+        <f>F10+1</f>
+        <v>44466</v>
+      </c>
+      <c r="F14" s="29">
+        <f>E14+3</f>
+        <v>44469</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
@@ -3443,8 +3471,8 @@
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
       <c r="W14" s="15"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
@@ -3488,29 +3516,29 @@
       <c r="BK14" s="15"/>
       <c r="BL14" s="15"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
-      <c r="B15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="14">
+      <c r="B15" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="35">
         <v>1</v>
       </c>
-      <c r="E15" s="29">
-        <f>F14</f>
+      <c r="E15" s="36">
+        <f>F14+1</f>
         <v>44470</v>
       </c>
-      <c r="F15" s="29">
-        <f>E15+3</f>
-        <v>44473</v>
+      <c r="F15" s="36">
+        <f>E15</f>
+        <v>44470</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
@@ -3569,29 +3597,29 @@
       <c r="BK15" s="15"/>
       <c r="BL15" s="15"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18"/>
       <c r="B16" s="24" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
       </c>
       <c r="E16" s="29">
-        <f>E15+1</f>
-        <v>44471</v>
+        <f>F15</f>
+        <v>44470</v>
       </c>
       <c r="F16" s="29">
-        <f>E16+6</f>
-        <v>44477</v>
+        <f>E16+3</f>
+        <v>44473</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
@@ -3650,21 +3678,29 @@
       <c r="BK16" s="15"/>
       <c r="BL16" s="15"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18"/>
+      <c r="B17" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29">
+        <f>E16+1</f>
+        <v>44471</v>
+      </c>
+      <c r="F17" s="29">
+        <f>E17+6</f>
+        <v>44477</v>
+      </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="13" t="str">
+      <c r="H17" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
@@ -3723,29 +3759,21 @@
       <c r="BK17" s="15"/>
       <c r="BL17" s="15"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="14">
-        <v>1</v>
-      </c>
-      <c r="E18" s="29">
-        <f>F16+1</f>
-        <v>44478</v>
-      </c>
-      <c r="F18" s="29">
-        <f>E18+9</f>
-        <v>44487</v>
-      </c>
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="13">
+      <c r="H18" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -3804,10 +3832,10 @@
       <c r="BK18" s="15"/>
       <c r="BL18" s="15"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18"/>
       <c r="B19" s="24" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>26</v>
@@ -3816,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="29">
-        <f>F16+1</f>
+        <f>F17+1</f>
         <v>44478</v>
       </c>
       <c r="F19" s="29">
@@ -3824,7 +3852,10 @@
         <v>44487</v>
       </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -3882,30 +3913,27 @@
       <c r="BK19" s="15"/>
       <c r="BL19" s="15"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18"/>
       <c r="B20" s="24" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="14">
         <v>1</v>
       </c>
       <c r="E20" s="29">
-        <f>F16+1</f>
+        <f>F17+1</f>
         <v>44478</v>
       </c>
       <c r="F20" s="29">
-        <f>E20+7</f>
-        <v>44485</v>
+        <f>E20+9</f>
+        <v>44487</v>
       </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="13">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
+      <c r="H20" s="13"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -3963,29 +3991,29 @@
       <c r="BK20" s="15"/>
       <c r="BL20" s="15"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D21" s="14">
         <v>1</v>
       </c>
       <c r="E21" s="29">
-        <f>F16+1</f>
+        <f>F17+1</f>
         <v>44478</v>
       </c>
       <c r="F21" s="29">
-        <f>E21+4</f>
-        <v>44482</v>
+        <f>E21+7</f>
+        <v>44485</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -4044,29 +4072,29 @@
       <c r="BK21" s="15"/>
       <c r="BL21" s="15"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18"/>
-      <c r="B22" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="35">
+      <c r="B22" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="14">
         <v>1</v>
       </c>
-      <c r="E22" s="36">
-        <f>E14+18</f>
-        <v>44488</v>
-      </c>
-      <c r="F22" s="36">
-        <f>E22</f>
-        <v>44488</v>
+      <c r="E22" s="29">
+        <f>F17+1</f>
+        <v>44478</v>
+      </c>
+      <c r="F22" s="29">
+        <f>E22+4</f>
+        <v>44482</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -4125,29 +4153,29 @@
       <c r="BK22" s="15"/>
       <c r="BL22" s="15"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18"/>
-      <c r="B23" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="14">
+      <c r="B23" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="35">
         <v>1</v>
       </c>
-      <c r="E23" s="29">
-        <f>F22</f>
+      <c r="E23" s="36">
+        <f>E15+18</f>
         <v>44488</v>
       </c>
-      <c r="F23" s="29">
-        <f>E23+6</f>
-        <v>44494</v>
+      <c r="F23" s="36">
+        <f>E23</f>
+        <v>44488</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -4206,29 +4234,29 @@
       <c r="BK23" s="15"/>
       <c r="BL23" s="15"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18"/>
       <c r="B24" s="24" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
       </c>
       <c r="E24" s="29">
-        <f>E23+1</f>
-        <v>44489</v>
+        <f>F23</f>
+        <v>44488</v>
       </c>
       <c r="F24" s="29">
-        <f>E24+11</f>
-        <v>44500</v>
+        <f>E24+6</f>
+        <v>44494</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -4287,29 +4315,29 @@
       <c r="BK24" s="15"/>
       <c r="BL24" s="15"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18"/>
       <c r="B25" s="24" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" s="14">
         <v>1</v>
       </c>
       <c r="E25" s="29">
-        <f>E23+1</f>
+        <f>E24+1</f>
         <v>44489</v>
       </c>
       <c r="F25" s="29">
-        <f>E25+15</f>
-        <v>44504</v>
+        <f>E25+11</f>
+        <v>44500</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -4368,19 +4396,19 @@
       <c r="BK25" s="15"/>
       <c r="BL25" s="15"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18"/>
       <c r="B26" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
       </c>
       <c r="E26" s="29">
-        <f>E23+1</f>
+        <f>E24+1</f>
         <v>44489</v>
       </c>
       <c r="F26" s="29">
@@ -4449,27 +4477,30 @@
       <c r="BK26" s="15"/>
       <c r="BL26" s="15"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
-      <c r="B27" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="35">
+      <c r="B27" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="14">
         <v>1</v>
       </c>
-      <c r="E27" s="36">
-        <f>F26+1</f>
-        <v>44505</v>
-      </c>
-      <c r="F27" s="36">
-        <f>E27</f>
-        <v>44505</v>
+      <c r="E27" s="29">
+        <f>E24+1</f>
+        <v>44489</v>
+      </c>
+      <c r="F27" s="29">
+        <f>E27+15</f>
+        <v>44504</v>
       </c>
       <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="13">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
@@ -4527,22 +4558,27 @@
       <c r="BK27" s="15"/>
       <c r="BL27" s="15"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="18"/>
+      <c r="B28" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="35">
+        <v>1</v>
+      </c>
+      <c r="E28" s="36">
+        <f>F27+1</f>
+        <v>44505</v>
+      </c>
+      <c r="F28" s="36">
+        <f>E28</f>
+        <v>44505</v>
+      </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H28" s="13"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
@@ -4600,29 +4636,21 @@
       <c r="BK28" s="15"/>
       <c r="BL28" s="15"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="18"/>
-      <c r="B29" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="14">
-        <v>1</v>
-      </c>
-      <c r="E29" s="29">
-        <f>F27</f>
-        <v>44505</v>
-      </c>
-      <c r="F29" s="29">
-        <f>E29+3</f>
-        <v>44508</v>
-      </c>
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="13">
+      <c r="H29" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -4681,29 +4709,29 @@
       <c r="BK29" s="15"/>
       <c r="BL29" s="15"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D30" s="14">
         <v>1</v>
       </c>
       <c r="E30" s="29">
-        <f>E29+1</f>
-        <v>44506</v>
+        <f>F28</f>
+        <v>44505</v>
       </c>
       <c r="F30" s="29">
-        <f>E30+2</f>
+        <f>E30+3</f>
         <v>44508</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -4762,29 +4790,29 @@
       <c r="BK30" s="15"/>
       <c r="BL30" s="15"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
       <c r="B31" s="24" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D31" s="14">
         <v>1</v>
       </c>
       <c r="E31" s="29">
-        <f>F30</f>
+        <f>E30+1</f>
+        <v>44506</v>
+      </c>
+      <c r="F31" s="29">
+        <f>E31+2</f>
         <v>44508</v>
-      </c>
-      <c r="F31" s="29">
-        <f>E31+6</f>
-        <v>44514</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -4843,29 +4871,29 @@
       <c r="BK31" s="15"/>
       <c r="BL31" s="15"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="24" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D32" s="14">
         <v>1</v>
       </c>
       <c r="E32" s="29">
-        <f>F31+1</f>
-        <v>44515</v>
+        <f>F31</f>
+        <v>44508</v>
       </c>
       <c r="F32" s="29">
-        <f>E32+9</f>
-        <v>44524</v>
+        <f>E32+6</f>
+        <v>44514</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -4924,29 +4952,29 @@
       <c r="BK32" s="15"/>
       <c r="BL32" s="15"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18"/>
       <c r="B33" s="24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D33" s="14">
         <v>1</v>
       </c>
       <c r="E33" s="29">
-        <f>F31+1</f>
+        <f>F32+1</f>
         <v>44515</v>
       </c>
       <c r="F33" s="29">
-        <f>E33+6</f>
-        <v>44521</v>
+        <f>E33+9</f>
+        <v>44524</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
@@ -5005,27 +5033,30 @@
       <c r="BK33" s="15"/>
       <c r="BL33" s="15"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18"/>
       <c r="B34" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" s="14">
         <v>1</v>
       </c>
       <c r="E34" s="29">
-        <f>F31+1</f>
+        <f>F32+1</f>
         <v>44515</v>
       </c>
       <c r="F34" s="29">
-        <f>E34+10</f>
-        <v>44525</v>
+        <f>E34+6</f>
+        <v>44521</v>
       </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -5083,30 +5114,27 @@
       <c r="BK34" s="15"/>
       <c r="BL34" s="15"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
-      <c r="B35" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="35">
+      <c r="B35" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="14">
         <v>1</v>
       </c>
-      <c r="E35" s="36">
-        <f>E27+21</f>
-        <v>44526</v>
-      </c>
-      <c r="F35" s="36">
-        <f>E35</f>
-        <v>44526</v>
+      <c r="E35" s="29">
+        <f>F32+1</f>
+        <v>44515</v>
+      </c>
+      <c r="F35" s="29">
+        <f>E35+10</f>
+        <v>44525</v>
       </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H35" s="13"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -5164,21 +5192,29 @@
       <c r="BK35" s="15"/>
       <c r="BL35" s="15"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="18"/>
+      <c r="B36" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="35">
+        <v>1</v>
+      </c>
+      <c r="E36" s="36">
+        <f>E28+21</f>
+        <v>44526</v>
+      </c>
+      <c r="F36" s="36">
+        <f>E36</f>
+        <v>44526</v>
+      </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="13" t="str">
+      <c r="H36" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
@@ -5237,29 +5273,21 @@
       <c r="BK36" s="15"/>
       <c r="BL36" s="15"/>
     </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="18"/>
-      <c r="B37" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1</v>
-      </c>
-      <c r="E37" s="29">
-        <f>F35+1</f>
-        <v>44527</v>
-      </c>
-      <c r="F37" s="29">
-        <f>E37+2</f>
-        <v>44529</v>
-      </c>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="13">
+      <c r="H37" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
@@ -5318,29 +5346,29 @@
       <c r="BK37" s="15"/>
       <c r="BL37" s="15"/>
     </row>
-    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18"/>
       <c r="B38" s="24" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D38" s="14">
         <v>1</v>
       </c>
       <c r="E38" s="29">
-        <f>E37+1</f>
-        <v>44528</v>
+        <f>F36+1</f>
+        <v>44527</v>
       </c>
       <c r="F38" s="29">
-        <f>E41-1</f>
-        <v>44546</v>
+        <f>E38+2</f>
+        <v>44529</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
@@ -5399,23 +5427,23 @@
       <c r="BK38" s="15"/>
       <c r="BL38" s="15"/>
     </row>
-    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
       <c r="B39" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E39" s="29">
-        <f>E38</f>
+        <f>E38+1</f>
         <v>44528</v>
       </c>
       <c r="F39" s="29">
-        <f>F38</f>
+        <f>E42-1</f>
         <v>44546</v>
       </c>
       <c r="G39" s="13"/>
@@ -5480,16 +5508,16 @@
       <c r="BK39" s="15"/>
       <c r="BL39" s="15"/>
     </row>
-    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18"/>
       <c r="B40" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D40" s="14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E40" s="29">
         <f>E39</f>
@@ -5500,7 +5528,10 @@
         <v>44546</v>
       </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="H40" s="13">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
@@ -5558,30 +5589,27 @@
       <c r="BK40" s="15"/>
       <c r="BL40" s="15"/>
     </row>
-    <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18"/>
-      <c r="B41" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" s="35">
+      <c r="B41" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="14">
         <v>1</v>
       </c>
-      <c r="E41" s="36">
-        <f>E35+21</f>
-        <v>44547</v>
-      </c>
-      <c r="F41" s="36">
-        <f>E41</f>
-        <v>44547</v>
+      <c r="E41" s="29">
+        <f>E40</f>
+        <v>44528</v>
+      </c>
+      <c r="F41" s="29">
+        <f>F40</f>
+        <v>44546</v>
       </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H41" s="13"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
@@ -5639,21 +5667,29 @@
       <c r="BK41" s="15"/>
       <c r="BL41" s="15"/>
     </row>
-    <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18"/>
+      <c r="B42" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="35">
+        <v>1</v>
+      </c>
+      <c r="E42" s="36">
+        <f>E36+21</f>
+        <v>44547</v>
+      </c>
+      <c r="F42" s="36">
+        <f>E42</f>
+        <v>44547</v>
+      </c>
       <c r="G42" s="13"/>
-      <c r="H42" s="13" t="str">
+      <c r="H42" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -5712,29 +5748,21 @@
       <c r="BK42" s="15"/>
       <c r="BL42" s="15"/>
     </row>
-    <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="18"/>
-      <c r="B43" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="14">
-        <v>1</v>
-      </c>
-      <c r="E43" s="29">
-        <f>E41</f>
-        <v>44547</v>
-      </c>
-      <c r="F43" s="29">
-        <f>E43+1</f>
-        <v>44548</v>
-      </c>
+    <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="38"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="13">
+      <c r="H43" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -5793,29 +5821,29 @@
       <c r="BK43" s="15"/>
       <c r="BL43" s="15"/>
     </row>
-    <row r="44" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
-      <c r="B44" s="32" t="s">
-        <v>55</v>
+      <c r="B44" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D44" s="14">
         <v>1</v>
       </c>
       <c r="E44" s="29">
-        <f>F43+1</f>
-        <v>44549</v>
+        <f>E42</f>
+        <v>44547</v>
       </c>
       <c r="F44" s="29">
-        <f>E44+7</f>
-        <v>44556</v>
+        <f>E44+1</f>
+        <v>44548</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
@@ -5874,29 +5902,29 @@
       <c r="BK44" s="15"/>
       <c r="BL44" s="15"/>
     </row>
-    <row r="45" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
-      <c r="B45" s="24" t="s">
-        <v>92</v>
+      <c r="B45" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D45" s="14">
         <v>1</v>
       </c>
       <c r="E45" s="29">
-        <f>F44</f>
+        <f>F44+1</f>
+        <v>44549</v>
+      </c>
+      <c r="F45" s="29">
+        <f>E45+7</f>
         <v>44556</v>
-      </c>
-      <c r="F45" s="29">
-        <f>E47-1</f>
-        <v>44585</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
@@ -5955,29 +5983,29 @@
       <c r="BK45" s="15"/>
       <c r="BL45" s="15"/>
     </row>
-    <row r="46" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18"/>
       <c r="B46" s="24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D46" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E46" s="29">
-        <f>F43+1</f>
-        <v>44549</v>
+        <f>F45</f>
+        <v>44556</v>
       </c>
       <c r="F46" s="29">
-        <f>E47-1</f>
+        <f>E48-1</f>
         <v>44585</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
@@ -6036,29 +6064,29 @@
       <c r="BK46" s="15"/>
       <c r="BL46" s="15"/>
     </row>
-    <row r="47" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18"/>
-      <c r="B47" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="35">
-        <v>1</v>
-      </c>
-      <c r="E47" s="36">
-        <f>E41+39</f>
-        <v>44586</v>
-      </c>
-      <c r="F47" s="36">
-        <f>E47</f>
-        <v>44586</v>
+      <c r="B47" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="E47" s="29">
+        <f>F44+1</f>
+        <v>44549</v>
+      </c>
+      <c r="F47" s="29">
+        <f>E48-1</f>
+        <v>44585</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -6117,21 +6145,29 @@
       <c r="BK47" s="15"/>
       <c r="BL47" s="15"/>
     </row>
-    <row r="48" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="38"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
+    <row r="48" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="18"/>
+      <c r="B48" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="35">
+        <v>1</v>
+      </c>
+      <c r="E48" s="36">
+        <f>E42+39</f>
+        <v>44586</v>
+      </c>
+      <c r="F48" s="36">
+        <f>E48</f>
+        <v>44586</v>
+      </c>
       <c r="G48" s="13"/>
-      <c r="H48" s="13" t="str">
+      <c r="H48" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
@@ -6190,27 +6226,21 @@
       <c r="BK48" s="15"/>
       <c r="BL48" s="15"/>
     </row>
-    <row r="49" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="18"/>
-      <c r="B49" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="14">
-        <v>1</v>
-      </c>
-      <c r="E49" s="29">
-        <f>F47+1</f>
-        <v>44587</v>
-      </c>
-      <c r="F49" s="29">
-        <f>E49</f>
-        <v>44587</v>
-      </c>
+    <row r="49" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="38"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
       <c r="G49" s="13"/>
-      <c r="H49" s="13">
+      <c r="H49" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
@@ -6269,29 +6299,27 @@
       <c r="BK49" s="15"/>
       <c r="BL49" s="15"/>
     </row>
-    <row r="50" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18"/>
       <c r="B50" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>26</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C50" s="22"/>
       <c r="D50" s="14">
         <v>1</v>
       </c>
       <c r="E50" s="29">
-        <f>F49+1</f>
-        <v>44588</v>
+        <f>F48+1</f>
+        <v>44587</v>
       </c>
       <c r="F50" s="29">
-        <f>E50+7</f>
-        <v>44595</v>
+        <f>E50</f>
+        <v>44587</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="13">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
@@ -6350,27 +6378,30 @@
       <c r="BK50" s="15"/>
       <c r="BL50" s="15"/>
     </row>
-    <row r="51" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18"/>
       <c r="B51" s="24" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="14">
         <v>1</v>
       </c>
       <c r="E51" s="29">
         <f>F50+1</f>
-        <v>44596</v>
+        <v>44588</v>
       </c>
       <c r="F51" s="29">
-        <f>E51+21</f>
-        <v>44617</v>
+        <f>E51+7</f>
+        <v>44595</v>
       </c>
       <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
+      <c r="H51" s="13">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -6428,23 +6459,23 @@
       <c r="BK51" s="15"/>
       <c r="BL51" s="15"/>
     </row>
-    <row r="52" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18"/>
       <c r="B52" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D52" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E52" s="29">
-        <f>E51</f>
+        <f>F51+1</f>
         <v>44596</v>
       </c>
       <c r="F52" s="29">
-        <f>F51</f>
+        <f>E52+21</f>
         <v>44617</v>
       </c>
       <c r="G52" s="13"/>
@@ -6506,16 +6537,16 @@
       <c r="BK52" s="15"/>
       <c r="BL52" s="15"/>
     </row>
-    <row r="53" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18"/>
       <c r="B53" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D53" s="14">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E53" s="29">
         <f>E52</f>
@@ -6584,23 +6615,23 @@
       <c r="BK53" s="15"/>
       <c r="BL53" s="15"/>
     </row>
-    <row r="54" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18"/>
       <c r="B54" s="24" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="D54" s="14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E54" s="29">
-        <f>F50+1</f>
+        <f>E53</f>
         <v>44596</v>
       </c>
       <c r="F54" s="29">
-        <f>E54+21</f>
+        <f>F53</f>
         <v>44617</v>
       </c>
       <c r="G54" s="13"/>
@@ -6662,24 +6693,24 @@
       <c r="BK54" s="15"/>
       <c r="BL54" s="15"/>
     </row>
-    <row r="55" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18"/>
       <c r="B55" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D55" s="14">
         <v>1</v>
       </c>
       <c r="E55" s="29">
-        <f>F54+1</f>
-        <v>44618</v>
+        <f>F51+1</f>
+        <v>44596</v>
       </c>
       <c r="F55" s="29">
-        <f>E55+4</f>
-        <v>44622</v>
+        <f>E55+21</f>
+        <v>44617</v>
       </c>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
@@ -6740,30 +6771,27 @@
       <c r="BK55" s="15"/>
       <c r="BL55" s="15"/>
     </row>
-    <row r="56" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18"/>
-      <c r="B56" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D56" s="35">
+      <c r="B56" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="14">
         <v>1</v>
       </c>
-      <c r="E56" s="36">
-        <f>F47+37</f>
-        <v>44623</v>
-      </c>
-      <c r="F56" s="36">
-        <f>E56</f>
-        <v>44623</v>
+      <c r="E56" s="29">
+        <f>F55+1</f>
+        <v>44618</v>
+      </c>
+      <c r="F56" s="29">
+        <f>E56+4</f>
+        <v>44622</v>
       </c>
       <c r="G56" s="13"/>
-      <c r="H56" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="H56" s="13"/>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
       <c r="K56" s="15"/>
@@ -6821,21 +6849,29 @@
       <c r="BK56" s="15"/>
       <c r="BL56" s="15"/>
     </row>
-    <row r="57" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="38"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
+    <row r="57" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="18"/>
+      <c r="B57" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="35">
+        <v>1</v>
+      </c>
+      <c r="E57" s="36">
+        <f>F48+37</f>
+        <v>44623</v>
+      </c>
+      <c r="F57" s="36">
+        <f>E57</f>
+        <v>44623</v>
+      </c>
       <c r="G57" s="13"/>
-      <c r="H57" s="13" t="str">
+      <c r="H57" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
@@ -6894,27 +6930,21 @@
       <c r="BK57" s="15"/>
       <c r="BL57" s="15"/>
     </row>
-    <row r="58" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="18"/>
-      <c r="B58" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" s="14">
-        <v>1</v>
-      </c>
-      <c r="E58" s="29">
-        <v>44624</v>
-      </c>
-      <c r="F58" s="29">
-        <v>44624</v>
-      </c>
+    <row r="58" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="38"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
       <c r="G58" s="13"/>
-      <c r="H58" s="13">
+      <c r="H58" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
@@ -6973,27 +7003,27 @@
       <c r="BK58" s="15"/>
       <c r="BL58" s="15"/>
     </row>
-    <row r="59" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18"/>
       <c r="B59" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="D59" s="14">
         <v>1</v>
       </c>
       <c r="E59" s="29">
-        <v>44625</v>
+        <v>44624</v>
       </c>
       <c r="F59" s="29">
-        <v>44631</v>
+        <v>44624</v>
       </c>
       <c r="G59" s="13"/>
       <c r="H59" s="13">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
@@ -7052,25 +7082,28 @@
       <c r="BK59" s="15"/>
       <c r="BL59" s="15"/>
     </row>
-    <row r="60" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18"/>
       <c r="B60" s="24" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D60" s="14">
         <v>1</v>
       </c>
       <c r="E60" s="29">
-        <v>44632</v>
+        <v>44625</v>
       </c>
       <c r="F60" s="29">
-        <v>44645</v>
+        <v>44631</v>
       </c>
       <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
+      <c r="H60" s="13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="I60" s="15"/>
       <c r="J60" s="15"/>
       <c r="K60" s="15"/>
@@ -7128,13 +7161,13 @@
       <c r="BK60" s="15"/>
       <c r="BL60" s="15"/>
     </row>
-    <row r="61" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18"/>
       <c r="B61" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="D61" s="14">
         <v>1</v>
@@ -7204,13 +7237,13 @@
       <c r="BK61" s="15"/>
       <c r="BL61" s="15"/>
     </row>
-    <row r="62" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18"/>
       <c r="B62" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="D62" s="14">
         <v>1</v>
@@ -7280,16 +7313,16 @@
       <c r="BK62" s="15"/>
       <c r="BL62" s="15"/>
     </row>
-    <row r="63" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18"/>
       <c r="B63" s="24" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="D63" s="14">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E63" s="29">
         <v>44632</v>
@@ -7298,10 +7331,7 @@
         <v>44645</v>
       </c>
       <c r="G63" s="13"/>
-      <c r="H63" s="13">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
+      <c r="H63" s="13"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
       <c r="K63" s="15"/>
@@ -7359,16 +7389,16 @@
       <c r="BK63" s="15"/>
       <c r="BL63" s="15"/>
     </row>
-    <row r="64" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18"/>
       <c r="B64" s="24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D64" s="14">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E64" s="29">
         <v>44632</v>
@@ -7377,7 +7407,10 @@
         <v>44645</v>
       </c>
       <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
+      <c r="H64" s="13">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
       <c r="K64" s="15"/>
@@ -7435,22 +7468,25 @@
       <c r="BK64" s="15"/>
       <c r="BL64" s="15"/>
     </row>
-    <row r="65" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="38"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
+    <row r="65" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="18"/>
+      <c r="B65" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E65" s="29">
+        <v>44632</v>
+      </c>
+      <c r="F65" s="29">
+        <v>44645</v>
+      </c>
       <c r="G65" s="13"/>
-      <c r="H65" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H65" s="13"/>
       <c r="I65" s="15"/>
       <c r="J65" s="15"/>
       <c r="K65" s="15"/>
@@ -7508,27 +7544,21 @@
       <c r="BK65" s="15"/>
       <c r="BL65" s="15"/>
     </row>
-    <row r="66" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="18"/>
-      <c r="B66" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D66" s="14">
-        <v>0</v>
-      </c>
-      <c r="E66" s="29">
-        <v>44646</v>
-      </c>
-      <c r="F66" s="29">
-        <v>44653</v>
-      </c>
+    <row r="66" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="38"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
       <c r="G66" s="13"/>
-      <c r="H66" s="13">
+      <c r="H66" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
@@ -7587,17 +7617,27 @@
       <c r="BK66" s="15"/>
       <c r="BL66" s="15"/>
     </row>
-    <row r="67" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
+      <c r="B67" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="14">
+        <v>0</v>
+      </c>
+      <c r="E67" s="29">
+        <v>44646</v>
+      </c>
+      <c r="F67" s="29">
+        <v>44646</v>
+      </c>
       <c r="G67" s="13"/>
-      <c r="H67" s="13" t="str">
+      <c r="H67" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I67" s="15"/>
       <c r="J67" s="15"/>
@@ -7656,29 +7696,25 @@
       <c r="BK67" s="15"/>
       <c r="BL67" s="15"/>
     </row>
-    <row r="68" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18"/>
-      <c r="B68" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D68" s="35">
+      <c r="B68" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" s="14">
         <v>0</v>
       </c>
-      <c r="E68" s="36">
-        <v>44655</v>
-      </c>
-      <c r="F68" s="36">
-        <f>E68+12</f>
-        <v>44667</v>
+      <c r="E68" s="29">
+        <v>44648</v>
+      </c>
+      <c r="F68" s="29">
+        <v>44651</v>
       </c>
       <c r="G68" s="13"/>
-      <c r="H68" s="13">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
+      <c r="H68" s="13"/>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
@@ -7736,22 +7772,25 @@
       <c r="BK68" s="15"/>
       <c r="BL68" s="15"/>
     </row>
-    <row r="69" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="38"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
+    <row r="69" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="18"/>
+      <c r="B69" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="14">
+        <v>0</v>
+      </c>
+      <c r="E69" s="29">
+        <v>44655</v>
+      </c>
+      <c r="F69" s="29">
+        <v>44662</v>
+      </c>
       <c r="G69" s="13"/>
-      <c r="H69" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H69" s="13"/>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>
       <c r="K69" s="15"/>
@@ -7809,22 +7848,25 @@
       <c r="BK69" s="15"/>
       <c r="BL69" s="15"/>
     </row>
-    <row r="70" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18"/>
       <c r="B70" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" s="22"/>
+        <v>98</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>72</v>
+      </c>
       <c r="D70" s="14">
-        <v>0</v>
-      </c>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
+        <v>0.4</v>
+      </c>
+      <c r="E70" s="29">
+        <v>44655</v>
+      </c>
+      <c r="F70" s="29">
+        <v>44659</v>
+      </c>
       <c r="G70" s="13"/>
-      <c r="H70" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H70" s="13"/>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
       <c r="K70" s="15"/>
@@ -7882,24 +7924,25 @@
       <c r="BK70" s="15"/>
       <c r="BL70" s="15"/>
     </row>
-    <row r="71" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18"/>
       <c r="B71" s="24" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="D71" s="14">
         <v>0</v>
       </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
+      <c r="E71" s="29">
+        <v>44657</v>
+      </c>
+      <c r="F71" s="29">
+        <v>44664</v>
+      </c>
       <c r="G71" s="13"/>
-      <c r="H71" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H71" s="13"/>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
       <c r="K71" s="15"/>
@@ -7957,18 +8000,25 @@
       <c r="BK71" s="15"/>
       <c r="BL71" s="15"/>
     </row>
-    <row r="72" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
+      <c r="B72" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E72" s="29">
+        <v>44651</v>
+      </c>
+      <c r="F72" s="29">
+        <v>44655</v>
+      </c>
       <c r="G72" s="13"/>
-      <c r="H72" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H72" s="13"/>
       <c r="I72" s="15"/>
       <c r="J72" s="15"/>
       <c r="K72" s="15"/>
@@ -8026,30 +8076,25 @@
       <c r="BK72" s="15"/>
       <c r="BL72" s="15"/>
     </row>
-    <row r="73" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="18"/>
-      <c r="B73" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C73" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D73" s="35">
-        <v>0</v>
-      </c>
-      <c r="E73" s="36">
-        <f>E68+35</f>
-        <v>44690</v>
-      </c>
-      <c r="F73" s="36">
-        <f>E73+12</f>
-        <v>44702</v>
+      <c r="B73" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="E73" s="29">
+        <v>44648</v>
+      </c>
+      <c r="F73" s="29">
+        <v>44662</v>
       </c>
       <c r="G73" s="13"/>
-      <c r="H73" s="13">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
+      <c r="H73" s="13"/>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
       <c r="K73" s="15"/>
@@ -8107,21 +8152,27 @@
       <c r="BK73" s="15"/>
       <c r="BL73" s="15"/>
     </row>
-    <row r="74" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" s="38"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
+    <row r="74" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="18"/>
+      <c r="B74" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="14">
+        <v>0</v>
+      </c>
+      <c r="E74" s="29">
+        <v>44662</v>
+      </c>
+      <c r="F74" s="29">
+        <v>44666</v>
+      </c>
       <c r="G74" s="13"/>
-      <c r="H74" s="13" t="str">
+      <c r="H74" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
@@ -8180,21 +8231,28 @@
       <c r="BK74" s="15"/>
       <c r="BL74" s="15"/>
     </row>
-    <row r="75" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="18"/>
-      <c r="B75" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="14">
+      <c r="B75" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="35">
         <v>0</v>
       </c>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
+      <c r="E75" s="36">
+        <v>44655</v>
+      </c>
+      <c r="F75" s="36">
+        <f>E75+12</f>
+        <v>44667</v>
+      </c>
       <c r="G75" s="13"/>
-      <c r="H75" s="13" t="str">
+      <c r="H75" s="13">
         <f t="shared" si="4"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="I75" s="15"/>
       <c r="J75" s="15"/>
@@ -8253,19 +8311,17 @@
       <c r="BK75" s="15"/>
       <c r="BL75" s="15"/>
     </row>
-    <row r="76" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="18"/>
-      <c r="B76" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D76" s="14">
-        <v>0</v>
-      </c>
-      <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
+    <row r="76" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="38"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13" t="str">
         <f t="shared" si="4"/>
@@ -8328,11 +8384,15 @@
       <c r="BK76" s="15"/>
       <c r="BL76" s="15"/>
     </row>
-    <row r="77" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="18"/>
-      <c r="B77" s="24"/>
+      <c r="B77" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="C77" s="22"/>
-      <c r="D77" s="14"/>
+      <c r="D77" s="14">
+        <v>0</v>
+      </c>
       <c r="E77" s="29"/>
       <c r="F77" s="29"/>
       <c r="G77" s="13"/>
@@ -8397,27 +8457,23 @@
       <c r="BK77" s="15"/>
       <c r="BL77" s="15"/>
     </row>
-    <row r="78" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="18"/>
-      <c r="B78" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" s="34" t="s">
+      <c r="B78" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D78" s="35"/>
-      <c r="E78" s="36">
-        <f>E73+5</f>
-        <v>44695</v>
-      </c>
-      <c r="F78" s="36">
-        <f>E78</f>
-        <v>44695</v>
-      </c>
+      <c r="D78" s="14">
+        <v>0</v>
+      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
       <c r="G78" s="13"/>
-      <c r="H78" s="13">
+      <c r="H78" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
@@ -8476,20 +8532,19 @@
       <c r="BK78" s="15"/>
       <c r="BL78" s="15"/>
     </row>
-    <row r="79" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
+    <row r="79" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="18"/>
+      <c r="B79" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="14">
+        <v>0</v>
+      </c>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
       <c r="G79" s="13"/>
-      <c r="H79" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H79" s="13"/>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
@@ -8547,15 +8602,752 @@
       <c r="BK79" s="15"/>
       <c r="BL79" s="15"/>
     </row>
-    <row r="80" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G80" s="6"/>
+    <row r="80" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="18"/>
+      <c r="B80" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="14">
+        <v>0</v>
+      </c>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
+      <c r="AA80" s="15"/>
+      <c r="AB80" s="15"/>
+      <c r="AC80" s="15"/>
+      <c r="AD80" s="15"/>
+      <c r="AE80" s="15"/>
+      <c r="AF80" s="15"/>
+      <c r="AG80" s="15"/>
+      <c r="AH80" s="15"/>
+      <c r="AI80" s="15"/>
+      <c r="AJ80" s="15"/>
+      <c r="AK80" s="15"/>
+      <c r="AL80" s="15"/>
+      <c r="AM80" s="15"/>
+      <c r="AN80" s="15"/>
+      <c r="AO80" s="15"/>
+      <c r="AP80" s="15"/>
+      <c r="AQ80" s="15"/>
+      <c r="AR80" s="15"/>
+      <c r="AS80" s="15"/>
+      <c r="AT80" s="15"/>
+      <c r="AU80" s="15"/>
+      <c r="AV80" s="15"/>
+      <c r="AW80" s="15"/>
+      <c r="AX80" s="15"/>
+      <c r="AY80" s="15"/>
+      <c r="AZ80" s="15"/>
+      <c r="BA80" s="15"/>
+      <c r="BB80" s="15"/>
+      <c r="BC80" s="15"/>
+      <c r="BD80" s="15"/>
+      <c r="BE80" s="15"/>
+      <c r="BF80" s="15"/>
+      <c r="BG80" s="15"/>
+      <c r="BH80" s="15"/>
+      <c r="BI80" s="15"/>
+      <c r="BJ80" s="15"/>
+      <c r="BK80" s="15"/>
+      <c r="BL80" s="15"/>
     </row>
-    <row r="81" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="10"/>
-      <c r="F81" s="20"/>
+    <row r="81" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="18"/>
+      <c r="B81" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D81" s="14">
+        <v>0</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="15"/>
+      <c r="V81" s="15"/>
+      <c r="W81" s="15"/>
+      <c r="X81" s="15"/>
+      <c r="Y81" s="15"/>
+      <c r="Z81" s="15"/>
+      <c r="AA81" s="15"/>
+      <c r="AB81" s="15"/>
+      <c r="AC81" s="15"/>
+      <c r="AD81" s="15"/>
+      <c r="AE81" s="15"/>
+      <c r="AF81" s="15"/>
+      <c r="AG81" s="15"/>
+      <c r="AH81" s="15"/>
+      <c r="AI81" s="15"/>
+      <c r="AJ81" s="15"/>
+      <c r="AK81" s="15"/>
+      <c r="AL81" s="15"/>
+      <c r="AM81" s="15"/>
+      <c r="AN81" s="15"/>
+      <c r="AO81" s="15"/>
+      <c r="AP81" s="15"/>
+      <c r="AQ81" s="15"/>
+      <c r="AR81" s="15"/>
+      <c r="AS81" s="15"/>
+      <c r="AT81" s="15"/>
+      <c r="AU81" s="15"/>
+      <c r="AV81" s="15"/>
+      <c r="AW81" s="15"/>
+      <c r="AX81" s="15"/>
+      <c r="AY81" s="15"/>
+      <c r="AZ81" s="15"/>
+      <c r="BA81" s="15"/>
+      <c r="BB81" s="15"/>
+      <c r="BC81" s="15"/>
+      <c r="BD81" s="15"/>
+      <c r="BE81" s="15"/>
+      <c r="BF81" s="15"/>
+      <c r="BG81" s="15"/>
+      <c r="BH81" s="15"/>
+      <c r="BI81" s="15"/>
+      <c r="BJ81" s="15"/>
+      <c r="BK81" s="15"/>
+      <c r="BL81" s="15"/>
     </row>
-    <row r="82" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C82" s="11"/>
+    <row r="82" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="18"/>
+      <c r="B82" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" s="35">
+        <v>0</v>
+      </c>
+      <c r="E82" s="36">
+        <f>E75+35</f>
+        <v>44690</v>
+      </c>
+      <c r="F82" s="36">
+        <f>E82+12</f>
+        <v>44702</v>
+      </c>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
+      <c r="V82" s="15"/>
+      <c r="W82" s="15"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="15"/>
+      <c r="Z82" s="15"/>
+      <c r="AA82" s="15"/>
+      <c r="AB82" s="15"/>
+      <c r="AC82" s="15"/>
+      <c r="AD82" s="15"/>
+      <c r="AE82" s="15"/>
+      <c r="AF82" s="15"/>
+      <c r="AG82" s="15"/>
+      <c r="AH82" s="15"/>
+      <c r="AI82" s="15"/>
+      <c r="AJ82" s="15"/>
+      <c r="AK82" s="15"/>
+      <c r="AL82" s="15"/>
+      <c r="AM82" s="15"/>
+      <c r="AN82" s="15"/>
+      <c r="AO82" s="15"/>
+      <c r="AP82" s="15"/>
+      <c r="AQ82" s="15"/>
+      <c r="AR82" s="15"/>
+      <c r="AS82" s="15"/>
+      <c r="AT82" s="15"/>
+      <c r="AU82" s="15"/>
+      <c r="AV82" s="15"/>
+      <c r="AW82" s="15"/>
+      <c r="AX82" s="15"/>
+      <c r="AY82" s="15"/>
+      <c r="AZ82" s="15"/>
+      <c r="BA82" s="15"/>
+      <c r="BB82" s="15"/>
+      <c r="BC82" s="15"/>
+      <c r="BD82" s="15"/>
+      <c r="BE82" s="15"/>
+      <c r="BF82" s="15"/>
+      <c r="BG82" s="15"/>
+      <c r="BH82" s="15"/>
+      <c r="BI82" s="15"/>
+      <c r="BJ82" s="15"/>
+      <c r="BK82" s="15"/>
+      <c r="BL82" s="15"/>
+    </row>
+    <row r="83" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C83" s="38"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="40"/>
+      <c r="F83" s="40"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
+      <c r="V83" s="15"/>
+      <c r="W83" s="15"/>
+      <c r="X83" s="15"/>
+      <c r="Y83" s="15"/>
+      <c r="Z83" s="15"/>
+      <c r="AA83" s="15"/>
+      <c r="AB83" s="15"/>
+      <c r="AC83" s="15"/>
+      <c r="AD83" s="15"/>
+      <c r="AE83" s="15"/>
+      <c r="AF83" s="15"/>
+      <c r="AG83" s="15"/>
+      <c r="AH83" s="15"/>
+      <c r="AI83" s="15"/>
+      <c r="AJ83" s="15"/>
+      <c r="AK83" s="15"/>
+      <c r="AL83" s="15"/>
+      <c r="AM83" s="15"/>
+      <c r="AN83" s="15"/>
+      <c r="AO83" s="15"/>
+      <c r="AP83" s="15"/>
+      <c r="AQ83" s="15"/>
+      <c r="AR83" s="15"/>
+      <c r="AS83" s="15"/>
+      <c r="AT83" s="15"/>
+      <c r="AU83" s="15"/>
+      <c r="AV83" s="15"/>
+      <c r="AW83" s="15"/>
+      <c r="AX83" s="15"/>
+      <c r="AY83" s="15"/>
+      <c r="AZ83" s="15"/>
+      <c r="BA83" s="15"/>
+      <c r="BB83" s="15"/>
+      <c r="BC83" s="15"/>
+      <c r="BD83" s="15"/>
+      <c r="BE83" s="15"/>
+      <c r="BF83" s="15"/>
+      <c r="BG83" s="15"/>
+      <c r="BH83" s="15"/>
+      <c r="BI83" s="15"/>
+      <c r="BJ83" s="15"/>
+      <c r="BK83" s="15"/>
+      <c r="BL83" s="15"/>
+    </row>
+    <row r="84" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="18"/>
+      <c r="B84" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C84" s="22"/>
+      <c r="D84" s="14">
+        <v>0</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15"/>
+      <c r="Q84" s="15"/>
+      <c r="R84" s="15"/>
+      <c r="S84" s="15"/>
+      <c r="T84" s="15"/>
+      <c r="U84" s="15"/>
+      <c r="V84" s="15"/>
+      <c r="W84" s="15"/>
+      <c r="X84" s="15"/>
+      <c r="Y84" s="15"/>
+      <c r="Z84" s="15"/>
+      <c r="AA84" s="15"/>
+      <c r="AB84" s="15"/>
+      <c r="AC84" s="15"/>
+      <c r="AD84" s="15"/>
+      <c r="AE84" s="15"/>
+      <c r="AF84" s="15"/>
+      <c r="AG84" s="15"/>
+      <c r="AH84" s="15"/>
+      <c r="AI84" s="15"/>
+      <c r="AJ84" s="15"/>
+      <c r="AK84" s="15"/>
+      <c r="AL84" s="15"/>
+      <c r="AM84" s="15"/>
+      <c r="AN84" s="15"/>
+      <c r="AO84" s="15"/>
+      <c r="AP84" s="15"/>
+      <c r="AQ84" s="15"/>
+      <c r="AR84" s="15"/>
+      <c r="AS84" s="15"/>
+      <c r="AT84" s="15"/>
+      <c r="AU84" s="15"/>
+      <c r="AV84" s="15"/>
+      <c r="AW84" s="15"/>
+      <c r="AX84" s="15"/>
+      <c r="AY84" s="15"/>
+      <c r="AZ84" s="15"/>
+      <c r="BA84" s="15"/>
+      <c r="BB84" s="15"/>
+      <c r="BC84" s="15"/>
+      <c r="BD84" s="15"/>
+      <c r="BE84" s="15"/>
+      <c r="BF84" s="15"/>
+      <c r="BG84" s="15"/>
+      <c r="BH84" s="15"/>
+      <c r="BI84" s="15"/>
+      <c r="BJ84" s="15"/>
+      <c r="BK84" s="15"/>
+      <c r="BL84" s="15"/>
+    </row>
+    <row r="85" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="18"/>
+      <c r="B85" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="14">
+        <v>0</v>
+      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+      <c r="U85" s="15"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="15"/>
+      <c r="X85" s="15"/>
+      <c r="Y85" s="15"/>
+      <c r="Z85" s="15"/>
+      <c r="AA85" s="15"/>
+      <c r="AB85" s="15"/>
+      <c r="AC85" s="15"/>
+      <c r="AD85" s="15"/>
+      <c r="AE85" s="15"/>
+      <c r="AF85" s="15"/>
+      <c r="AG85" s="15"/>
+      <c r="AH85" s="15"/>
+      <c r="AI85" s="15"/>
+      <c r="AJ85" s="15"/>
+      <c r="AK85" s="15"/>
+      <c r="AL85" s="15"/>
+      <c r="AM85" s="15"/>
+      <c r="AN85" s="15"/>
+      <c r="AO85" s="15"/>
+      <c r="AP85" s="15"/>
+      <c r="AQ85" s="15"/>
+      <c r="AR85" s="15"/>
+      <c r="AS85" s="15"/>
+      <c r="AT85" s="15"/>
+      <c r="AU85" s="15"/>
+      <c r="AV85" s="15"/>
+      <c r="AW85" s="15"/>
+      <c r="AX85" s="15"/>
+      <c r="AY85" s="15"/>
+      <c r="AZ85" s="15"/>
+      <c r="BA85" s="15"/>
+      <c r="BB85" s="15"/>
+      <c r="BC85" s="15"/>
+      <c r="BD85" s="15"/>
+      <c r="BE85" s="15"/>
+      <c r="BF85" s="15"/>
+      <c r="BG85" s="15"/>
+      <c r="BH85" s="15"/>
+      <c r="BI85" s="15"/>
+      <c r="BJ85" s="15"/>
+      <c r="BK85" s="15"/>
+      <c r="BL85" s="15"/>
+    </row>
+    <row r="86" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="18"/>
+      <c r="B86" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="14">
+        <v>0</v>
+      </c>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
+      <c r="U86" s="15"/>
+      <c r="V86" s="15"/>
+      <c r="W86" s="15"/>
+      <c r="X86" s="15"/>
+      <c r="Y86" s="15"/>
+      <c r="Z86" s="15"/>
+      <c r="AA86" s="15"/>
+      <c r="AB86" s="15"/>
+      <c r="AC86" s="15"/>
+      <c r="AD86" s="15"/>
+      <c r="AE86" s="15"/>
+      <c r="AF86" s="15"/>
+      <c r="AG86" s="15"/>
+      <c r="AH86" s="15"/>
+      <c r="AI86" s="15"/>
+      <c r="AJ86" s="15"/>
+      <c r="AK86" s="15"/>
+      <c r="AL86" s="15"/>
+      <c r="AM86" s="15"/>
+      <c r="AN86" s="15"/>
+      <c r="AO86" s="15"/>
+      <c r="AP86" s="15"/>
+      <c r="AQ86" s="15"/>
+      <c r="AR86" s="15"/>
+      <c r="AS86" s="15"/>
+      <c r="AT86" s="15"/>
+      <c r="AU86" s="15"/>
+      <c r="AV86" s="15"/>
+      <c r="AW86" s="15"/>
+      <c r="AX86" s="15"/>
+      <c r="AY86" s="15"/>
+      <c r="AZ86" s="15"/>
+      <c r="BA86" s="15"/>
+      <c r="BB86" s="15"/>
+      <c r="BC86" s="15"/>
+      <c r="BD86" s="15"/>
+      <c r="BE86" s="15"/>
+      <c r="BF86" s="15"/>
+      <c r="BG86" s="15"/>
+      <c r="BH86" s="15"/>
+      <c r="BI86" s="15"/>
+      <c r="BJ86" s="15"/>
+      <c r="BK86" s="15"/>
+      <c r="BL86" s="15"/>
+    </row>
+    <row r="87" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="18"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="15"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="15"/>
+      <c r="V87" s="15"/>
+      <c r="W87" s="15"/>
+      <c r="X87" s="15"/>
+      <c r="Y87" s="15"/>
+      <c r="Z87" s="15"/>
+      <c r="AA87" s="15"/>
+      <c r="AB87" s="15"/>
+      <c r="AC87" s="15"/>
+      <c r="AD87" s="15"/>
+      <c r="AE87" s="15"/>
+      <c r="AF87" s="15"/>
+      <c r="AG87" s="15"/>
+      <c r="AH87" s="15"/>
+      <c r="AI87" s="15"/>
+      <c r="AJ87" s="15"/>
+      <c r="AK87" s="15"/>
+      <c r="AL87" s="15"/>
+      <c r="AM87" s="15"/>
+      <c r="AN87" s="15"/>
+      <c r="AO87" s="15"/>
+      <c r="AP87" s="15"/>
+      <c r="AQ87" s="15"/>
+      <c r="AR87" s="15"/>
+      <c r="AS87" s="15"/>
+      <c r="AT87" s="15"/>
+      <c r="AU87" s="15"/>
+      <c r="AV87" s="15"/>
+      <c r="AW87" s="15"/>
+      <c r="AX87" s="15"/>
+      <c r="AY87" s="15"/>
+      <c r="AZ87" s="15"/>
+      <c r="BA87" s="15"/>
+      <c r="BB87" s="15"/>
+      <c r="BC87" s="15"/>
+      <c r="BD87" s="15"/>
+      <c r="BE87" s="15"/>
+      <c r="BF87" s="15"/>
+      <c r="BG87" s="15"/>
+      <c r="BH87" s="15"/>
+      <c r="BI87" s="15"/>
+      <c r="BJ87" s="15"/>
+      <c r="BK87" s="15"/>
+      <c r="BL87" s="15"/>
+    </row>
+    <row r="88" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="18"/>
+      <c r="B88" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" s="35"/>
+      <c r="E88" s="36">
+        <f>E82+5</f>
+        <v>44695</v>
+      </c>
+      <c r="F88" s="36">
+        <f>E88</f>
+        <v>44695</v>
+      </c>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="15"/>
+      <c r="U88" s="15"/>
+      <c r="V88" s="15"/>
+      <c r="W88" s="15"/>
+      <c r="X88" s="15"/>
+      <c r="Y88" s="15"/>
+      <c r="Z88" s="15"/>
+      <c r="AA88" s="15"/>
+      <c r="AB88" s="15"/>
+      <c r="AC88" s="15"/>
+      <c r="AD88" s="15"/>
+      <c r="AE88" s="15"/>
+      <c r="AF88" s="15"/>
+      <c r="AG88" s="15"/>
+      <c r="AH88" s="15"/>
+      <c r="AI88" s="15"/>
+      <c r="AJ88" s="15"/>
+      <c r="AK88" s="15"/>
+      <c r="AL88" s="15"/>
+      <c r="AM88" s="15"/>
+      <c r="AN88" s="15"/>
+      <c r="AO88" s="15"/>
+      <c r="AP88" s="15"/>
+      <c r="AQ88" s="15"/>
+      <c r="AR88" s="15"/>
+      <c r="AS88" s="15"/>
+      <c r="AT88" s="15"/>
+      <c r="AU88" s="15"/>
+      <c r="AV88" s="15"/>
+      <c r="AW88" s="15"/>
+      <c r="AX88" s="15"/>
+      <c r="AY88" s="15"/>
+      <c r="AZ88" s="15"/>
+      <c r="BA88" s="15"/>
+      <c r="BB88" s="15"/>
+      <c r="BC88" s="15"/>
+      <c r="BD88" s="15"/>
+      <c r="BE88" s="15"/>
+      <c r="BF88" s="15"/>
+      <c r="BG88" s="15"/>
+      <c r="BH88" s="15"/>
+      <c r="BI88" s="15"/>
+      <c r="BJ88" s="15"/>
+      <c r="BK88" s="15"/>
+      <c r="BL88" s="15"/>
+    </row>
+    <row r="89" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" s="25"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="15"/>
+      <c r="O89" s="15"/>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="15"/>
+      <c r="R89" s="15"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="15"/>
+      <c r="U89" s="15"/>
+      <c r="V89" s="15"/>
+      <c r="W89" s="15"/>
+      <c r="X89" s="15"/>
+      <c r="Y89" s="15"/>
+      <c r="Z89" s="15"/>
+      <c r="AA89" s="15"/>
+      <c r="AB89" s="15"/>
+      <c r="AC89" s="15"/>
+      <c r="AD89" s="15"/>
+      <c r="AE89" s="15"/>
+      <c r="AF89" s="15"/>
+      <c r="AG89" s="15"/>
+      <c r="AH89" s="15"/>
+      <c r="AI89" s="15"/>
+      <c r="AJ89" s="15"/>
+      <c r="AK89" s="15"/>
+      <c r="AL89" s="15"/>
+      <c r="AM89" s="15"/>
+      <c r="AN89" s="15"/>
+      <c r="AO89" s="15"/>
+      <c r="AP89" s="15"/>
+      <c r="AQ89" s="15"/>
+      <c r="AR89" s="15"/>
+      <c r="AS89" s="15"/>
+      <c r="AT89" s="15"/>
+      <c r="AU89" s="15"/>
+      <c r="AV89" s="15"/>
+      <c r="AW89" s="15"/>
+      <c r="AX89" s="15"/>
+      <c r="AY89" s="15"/>
+      <c r="AZ89" s="15"/>
+      <c r="BA89" s="15"/>
+      <c r="BB89" s="15"/>
+      <c r="BC89" s="15"/>
+      <c r="BD89" s="15"/>
+      <c r="BE89" s="15"/>
+      <c r="BF89" s="15"/>
+      <c r="BG89" s="15"/>
+      <c r="BH89" s="15"/>
+      <c r="BI89" s="15"/>
+      <c r="BJ89" s="15"/>
+      <c r="BK89" s="15"/>
+      <c r="BL89" s="15"/>
+    </row>
+    <row r="90" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G90" s="6"/>
+    </row>
+    <row r="91" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="10"/>
+      <c r="F91" s="20"/>
+    </row>
+    <row r="92" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -8573,7 +9365,7 @@
     <mergeCell ref="AK5:AQ5"/>
     <mergeCell ref="AR5:AX5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D15:D16 D79 D23:D26 D18:D21 D66:D67 D49:D55">
+  <conditionalFormatting sqref="D16:D17 D89 D24:D27 D19:D22 D50:D56 D67:D74">
     <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8587,12 +9379,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79:BL79 I33:BL35 I6:BL26 I28:BL30 I65:BL67 I48:BL55">
+  <conditionalFormatting sqref="I89:BL89 I34:BL36 I6:BL27 I29:BL31 I66:BL74 I49:BL56">
     <cfRule type="expression" dxfId="50" priority="124">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79:BL79 I33:BL35 I8:BL26 I28:BL30 I65:BL67 I48:BL55">
+  <conditionalFormatting sqref="I89:BL89 I34:BL36 I8:BL27 I29:BL31 I66:BL74 I49:BL56">
     <cfRule type="expression" dxfId="49" priority="122">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8600,7 +9392,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D34 D29:D30">
+  <conditionalFormatting sqref="D34:D35 D30:D31">
     <cfRule type="dataBar" priority="120">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8614,7 +9406,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="D47">
     <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8628,12 +9420,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:BL44 I46:BL46">
+  <conditionalFormatting sqref="I43:BL45 I47:BL47">
     <cfRule type="expression" dxfId="47" priority="119">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:BL44 I46:BL46">
+  <conditionalFormatting sqref="I43:BL45 I47:BL47">
     <cfRule type="expression" dxfId="46" priority="117">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8641,7 +9433,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44">
+  <conditionalFormatting sqref="D44:D45">
     <cfRule type="dataBar" priority="115">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8655,12 +9447,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47">
+  <conditionalFormatting sqref="I48:BL48">
     <cfRule type="expression" dxfId="44" priority="113">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47">
+  <conditionalFormatting sqref="I48:BL48">
     <cfRule type="expression" dxfId="43" priority="111">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8668,12 +9460,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL56">
+  <conditionalFormatting sqref="I57:BL57">
     <cfRule type="expression" dxfId="41" priority="104">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL56">
+  <conditionalFormatting sqref="I57:BL57">
     <cfRule type="expression" dxfId="40" priority="102">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8681,7 +9473,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D64">
+  <conditionalFormatting sqref="D64:D65">
     <cfRule type="dataBar" priority="98">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8695,12 +9487,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:BL64">
+  <conditionalFormatting sqref="I58:BL65">
     <cfRule type="expression" dxfId="38" priority="101">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:BL64">
+  <conditionalFormatting sqref="I58:BL65">
     <cfRule type="expression" dxfId="37" priority="99">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8708,7 +9500,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58:D62">
+  <conditionalFormatting sqref="D59:D63">
     <cfRule type="dataBar" priority="97">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8722,7 +9514,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D13">
+  <conditionalFormatting sqref="D12:D14">
     <cfRule type="dataBar" priority="87">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8750,26 +9542,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
-    <cfRule type="dataBar" priority="80">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DEED8560-2EDB-4507-858D-EC48F4358421}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69:BL72">
+  <conditionalFormatting sqref="I76:BL81">
     <cfRule type="expression" dxfId="35" priority="83">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69:BL72">
+  <conditionalFormatting sqref="I76:BL81">
     <cfRule type="expression" dxfId="34" priority="81">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8777,12 +9555,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68:BL68">
+  <conditionalFormatting sqref="I75:BL75">
     <cfRule type="expression" dxfId="32" priority="79">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68:BL68">
+  <conditionalFormatting sqref="I75:BL75">
     <cfRule type="expression" dxfId="31" priority="77">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8790,7 +9568,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D71">
+  <conditionalFormatting sqref="D77:D81">
     <cfRule type="dataBar" priority="75">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8804,7 +9582,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D77">
+  <conditionalFormatting sqref="D87">
     <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8818,12 +9596,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I74:BL77">
+  <conditionalFormatting sqref="I83:BL87">
     <cfRule type="expression" dxfId="29" priority="73">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I74:BL77">
+  <conditionalFormatting sqref="I83:BL87">
     <cfRule type="expression" dxfId="28" priority="71">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8831,12 +9609,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73:BL73">
+  <conditionalFormatting sqref="I82:BL82">
     <cfRule type="expression" dxfId="26" priority="69">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73:BL73">
+  <conditionalFormatting sqref="I82:BL82">
     <cfRule type="expression" dxfId="25" priority="67">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8844,7 +9622,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75:D76">
+  <conditionalFormatting sqref="D84:D86">
     <cfRule type="dataBar" priority="65">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8858,12 +9636,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I78:BL78">
+  <conditionalFormatting sqref="I88:BL88">
     <cfRule type="expression" dxfId="23" priority="63">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I78:BL78">
+  <conditionalFormatting sqref="I88:BL88">
     <cfRule type="expression" dxfId="22" priority="61">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8871,12 +9649,12 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:BL31">
+  <conditionalFormatting sqref="I32:BL32">
     <cfRule type="expression" dxfId="20" priority="59">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:BL31">
+  <conditionalFormatting sqref="I32:BL32">
     <cfRule type="expression" dxfId="19" priority="57">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8884,7 +9662,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8898,12 +9676,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL32">
+  <conditionalFormatting sqref="I33:BL33">
     <cfRule type="expression" dxfId="17" priority="55">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL32">
+  <conditionalFormatting sqref="I33:BL33">
     <cfRule type="expression" dxfId="16" priority="53">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8911,7 +9689,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8925,12 +9703,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL37 I41:BL41">
+  <conditionalFormatting sqref="I37:BL38 I42:BL42">
     <cfRule type="expression" dxfId="14" priority="51">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL37 I41:BL41">
+  <conditionalFormatting sqref="I37:BL38 I42:BL42">
     <cfRule type="expression" dxfId="13" priority="49">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8938,7 +9716,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D38">
     <cfRule type="dataBar" priority="48">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8952,12 +9730,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL38">
+  <conditionalFormatting sqref="I39:BL39">
     <cfRule type="expression" dxfId="11" priority="47">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL38">
+  <conditionalFormatting sqref="I39:BL39">
     <cfRule type="expression" dxfId="10" priority="45">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8965,7 +9743,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
+  <conditionalFormatting sqref="D39">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8979,12 +9757,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:BL40">
+  <conditionalFormatting sqref="I40:BL41">
     <cfRule type="expression" dxfId="8" priority="43">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:BL40">
+  <conditionalFormatting sqref="I40:BL41">
     <cfRule type="expression" dxfId="7" priority="41">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -8992,7 +9770,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D40">
+  <conditionalFormatting sqref="D40:D41">
     <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9006,7 +9784,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="D46">
     <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9020,12 +9798,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45:BL45">
+  <conditionalFormatting sqref="I46:BL46">
     <cfRule type="expression" dxfId="5" priority="39">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45:BL45">
+  <conditionalFormatting sqref="I46:BL46">
     <cfRule type="expression" dxfId="4" priority="37">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -9061,7 +9839,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="D15">
     <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9075,7 +9853,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="D18">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9089,7 +9867,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
+  <conditionalFormatting sqref="D23">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9103,7 +9881,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9117,7 +9895,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="D42">
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9131,7 +9909,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D48">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9145,7 +9923,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9159,7 +9937,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
+  <conditionalFormatting sqref="D75">
     <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9173,7 +9951,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
+  <conditionalFormatting sqref="D82">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9187,7 +9965,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D78">
+  <conditionalFormatting sqref="D88">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9201,7 +9979,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
+  <conditionalFormatting sqref="D29">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9215,7 +9993,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9229,7 +10007,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9243,7 +10021,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D49">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9257,7 +10035,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="D58">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9271,7 +10049,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D66">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9285,7 +10063,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
+  <conditionalFormatting sqref="D76">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9299,7 +10077,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
+  <conditionalFormatting sqref="D83">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9313,12 +10091,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:BL27">
+  <conditionalFormatting sqref="I28:BL28">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:BL27">
+  <conditionalFormatting sqref="I28:BL28">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(début_tâche&lt;=I$6,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$6)</formula>
     </cfRule>
@@ -9326,7 +10104,7 @@
       <formula>AND(fin_tâche&gt;=I$6,début_tâche&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
+  <conditionalFormatting sqref="D28">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9367,7 +10145,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15:D16 D79 D23:D26 D18:D21 D66:D67 D49:D55</xm:sqref>
+          <xm:sqref>D16:D17 D89 D24:D27 D19:D22 D50:D56 D67:D74</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{61BAFCB1-C9D1-4453-9835-894AAFFB2D48}">
@@ -9382,7 +10160,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D33:D34 D29:D30</xm:sqref>
+          <xm:sqref>D34:D35 D30:D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AD57E977-98C8-4463-AF63-0B910B22A855}">
@@ -9397,7 +10175,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D46</xm:sqref>
+          <xm:sqref>D47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{85DD6914-E53C-41B0-AFBA-86F7B9451DA6}">
@@ -9412,7 +10190,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D43:D44</xm:sqref>
+          <xm:sqref>D44:D45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F7F63C90-679F-41E1-9DD7-C7641723B832}">
@@ -9427,7 +10205,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D63:D64</xm:sqref>
+          <xm:sqref>D64:D65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8C1F1D87-2F5D-4508-9015-0F4807608336}">
@@ -9442,7 +10220,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D58:D62</xm:sqref>
+          <xm:sqref>D59:D63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{85676472-4DEA-4B47-8076-2B079F7EB722}">
@@ -9457,7 +10235,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D12:D13</xm:sqref>
+          <xm:sqref>D12:D14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{31E90CF3-9F5F-44CA-B687-A51E64DCC915}">
@@ -9475,21 +10253,6 @@
           <xm:sqref>D10:D11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DEED8560-2EDB-4507-858D-EC48F4358421}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D72</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D92EFAD8-9A39-41D6-8E74-09FCB7C99446}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -9502,7 +10265,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D70:D71</xm:sqref>
+          <xm:sqref>D77:D81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{49690BEA-F1DA-49A9-87E0-BC10D33392B4}">
@@ -9517,7 +10280,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D77</xm:sqref>
+          <xm:sqref>D87</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F3BCBE8B-1131-4EC4-93C6-93A3D2241A3A}">
@@ -9532,7 +10295,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D75:D76</xm:sqref>
+          <xm:sqref>D84:D86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{70FE4911-65CD-4B63-902B-DAD573D9D1E7}">
@@ -9547,7 +10310,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D31</xm:sqref>
+          <xm:sqref>D32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{107B3D2A-9D99-4B77-A0C1-E7D4234EC328}">
@@ -9562,7 +10325,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4BDF0497-329E-4ACE-A091-C6666647B0A6}">
@@ -9577,7 +10340,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D37</xm:sqref>
+          <xm:sqref>D38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2616EACB-B142-4ABA-AB98-D0EFAE3192B1}">
@@ -9592,7 +10355,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D38</xm:sqref>
+          <xm:sqref>D39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9179826B-45ED-4988-BB2A-78DA7424E602}">
@@ -9607,7 +10370,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D39:D40</xm:sqref>
+          <xm:sqref>D40:D41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9795FCF7-A67A-433E-B155-AD1C0E7C374A}">
@@ -9622,7 +10385,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D45</xm:sqref>
+          <xm:sqref>D46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{36C8D48B-9FF9-4463-BC3F-14FABEE2DEF7}">
@@ -9667,7 +10430,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D14</xm:sqref>
+          <xm:sqref>D15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B4ED5E57-C950-47E4-A099-DCA192DFE477}">
@@ -9682,7 +10445,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D17</xm:sqref>
+          <xm:sqref>D18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{164A214E-470A-43CF-8C6A-55A5991E08E9}">
@@ -9697,7 +10460,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D22</xm:sqref>
+          <xm:sqref>D23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DE1AD479-0A37-44F4-AC20-51FF297665D3}">
@@ -9712,7 +10475,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{49FBE34D-D83B-497D-AB99-28B0686734FB}">
@@ -9727,7 +10490,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D41</xm:sqref>
+          <xm:sqref>D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FFA7516B-0875-4D87-99ED-B7E4CACCC0E1}">
@@ -9742,7 +10505,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D47</xm:sqref>
+          <xm:sqref>D48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{66BA6DFA-1489-4D78-8D16-D0BABA15730F}">
@@ -9757,7 +10520,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D56</xm:sqref>
+          <xm:sqref>D57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F9FF2D8E-4C48-4314-AE00-D91E4BEBF00D}">
@@ -9772,7 +10535,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D68</xm:sqref>
+          <xm:sqref>D75</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{47FD5541-751B-48F2-895B-231260031964}">
@@ -9787,7 +10550,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D73</xm:sqref>
+          <xm:sqref>D82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CB458C94-EC1D-48A0-8F37-BA38EE604418}">
@@ -9802,7 +10565,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D78</xm:sqref>
+          <xm:sqref>D88</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AC19E591-9826-41D2-8753-21A5AEC1982F}">
@@ -9817,7 +10580,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D28</xm:sqref>
+          <xm:sqref>D29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7E87486C-C83F-46B9-BB58-D6A8CEED9048}">
@@ -9832,7 +10595,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36</xm:sqref>
+          <xm:sqref>D37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1FF748D9-3BCB-4034-9208-1F2D65C79F13}">
@@ -9847,7 +10610,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D42</xm:sqref>
+          <xm:sqref>D43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F2C994C7-19E2-44FD-954A-AB7D6DE46441}">
@@ -9862,7 +10625,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D48</xm:sqref>
+          <xm:sqref>D49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8CA27610-5A3B-4302-BEA5-774F42E0EC59}">
@@ -9877,7 +10640,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D57</xm:sqref>
+          <xm:sqref>D58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B566DAE9-59F0-494F-B4A5-6CA202ED05AF}">
@@ -9892,7 +10655,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D65</xm:sqref>
+          <xm:sqref>D66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E8B7A00D-0A45-4E39-935E-0EF6E104B91A}">
@@ -9907,7 +10670,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D69</xm:sqref>
+          <xm:sqref>D76</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{61C46EA8-F9E7-45B9-92F2-CA890223D6D5}">
@@ -9922,7 +10685,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D74</xm:sqref>
+          <xm:sqref>D83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8A618AE5-6A10-402E-8877-7F8471EF9C36}">
@@ -9937,7 +10700,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D27</xm:sqref>
+          <xm:sqref>D28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>